<commit_message>
update change_log for 3.30.00.03
</commit_message>
<xml_diff>
--- a/SS_330_Change_Log.xlsx
+++ b/SS_330_Change_Log.xlsx
@@ -20,7 +20,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$3:$E$216</definedName>
     <definedName name="_xlnm.database">Sheet1!$A$3:$F$101</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
   <si>
     <t>Date</t>
   </si>
@@ -90,9 +90,6 @@
     <t>Updated:  10/31/2010</t>
   </si>
   <si>
-    <t>11/15/2016 for 3.30.00.02</t>
-  </si>
-  <si>
     <t>3.30.00.00</t>
   </si>
   <si>
@@ -121,6 +118,21 @@
   </si>
   <si>
     <t>fix missing write of length_maturity vector for maturity option 6</t>
+  </si>
+  <si>
+    <t>11/17/2016 for 3.30.00.03</t>
+  </si>
+  <si>
+    <t>3.30.00.03</t>
+  </si>
+  <si>
+    <t>read</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>fix Q parm count issue in ss_readcontrol_324</t>
   </si>
 </sst>
 </file>
@@ -556,7 +568,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
+      <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -578,7 +590,7 @@
         <v>8</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25"/>
@@ -605,10 +617,10 @@
     <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="8"/>
       <c r="B4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="9" t="s">
         <v>10</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -616,16 +628,16 @@
         <v>42683</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>14</v>
-      </c>
       <c r="F5" s="9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -633,24 +645,40 @@
         <v>42689</v>
       </c>
       <c r="B6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="5" t="s">
+      <c r="E6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="F6" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="9" t="s">
-        <v>19</v>
-      </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
-      <c r="F7" s="9"/>
+      <c r="A7" s="8">
+        <v>42691</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>

</xml_diff>

<commit_message>
3.30.01.00:  revise 3rd retention parameter from direct estimate on 0, 1 scale to logit:  1/(1+exp(-X)); convert with sstrans
</commit_message>
<xml_diff>
--- a/SS_330_Change_Log.xlsx
+++ b/SS_330_Change_Log.xlsx
@@ -20,7 +20,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$3:$E$216</definedName>
     <definedName name="_xlnm.database">Sheet1!$A$3:$F$101</definedName>
   </definedNames>
-  <calcPr calcId="145621" iterateDelta="1E-4"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
   <si>
     <t>Date</t>
   </si>
@@ -120,9 +120,6 @@
     <t>fix missing write of length_maturity vector for maturity option 6</t>
   </si>
   <si>
-    <t>11/17/2016 for 3.30.00.03</t>
-  </si>
-  <si>
     <t>3.30.00.03</t>
   </si>
   <si>
@@ -133,6 +130,24 @@
   </si>
   <si>
     <t>fix Q parm count issue in ss_readcontrol_324</t>
+  </si>
+  <si>
+    <t>3.30.01.00</t>
+  </si>
+  <si>
+    <t>revise</t>
+  </si>
+  <si>
+    <t>selectivity</t>
+  </si>
+  <si>
+    <t>retention</t>
+  </si>
+  <si>
+    <t>revise 3rd retention parameter from direct estimate on 0, 1 scale to logit:  1/(1+exp(-X)); convert with sstrans</t>
+  </si>
+  <si>
+    <t>11/22/2016 for 3.30.01.00</t>
   </si>
 </sst>
 </file>
@@ -568,7 +583,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
+      <selection pane="bottomLeft" activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -590,7 +605,7 @@
         <v>8</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25"/>
@@ -665,24 +680,40 @@
         <v>42691</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D7" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="F7" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="9" t="s">
+    </row>
+    <row r="8" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="8">
+        <v>42696</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
-      <c r="F8" s="9"/>
+      <c r="C8" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="8"/>

</xml_diff>

<commit_message>
VLAB #30394 data in forecast and VLAB #12960 timing of fishery samples;  3.30.02.00; add to change log
</commit_message>
<xml_diff>
--- a/SS_330_Change_Log.xlsx
+++ b/SS_330_Change_Log.xlsx
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="35">
   <si>
     <t>Date</t>
   </si>
@@ -147,7 +147,25 @@
     <t>revise 3rd retention parameter from direct estimate on 0, 1 scale to logit:  1/(1+exp(-X)); convert with sstrans</t>
   </si>
   <si>
-    <t>11/22/2016 for 3.30.01.00</t>
+    <t>3.30.01.15</t>
+  </si>
+  <si>
+    <t>various fixes implemented; see git for details.  Includes addition of truncated normal error for discard data</t>
+  </si>
+  <si>
+    <t>3.30.02.00</t>
+  </si>
+  <si>
+    <t>new</t>
+  </si>
+  <si>
+    <t>expected_values</t>
+  </si>
+  <si>
+    <t>add ability to have expected values in forecast; all data read after retroyr set to have no logL; also add explicit timing option (month&gt;1000) for fishery samples</t>
+  </si>
+  <si>
+    <t>04/13/2017 for 3.30.02.00</t>
   </si>
 </sst>
 </file>
@@ -583,7 +601,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
+      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -605,7 +623,7 @@
         <v>8</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25"/>
@@ -715,13 +733,39 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
-      <c r="F9" s="9"/>
-    </row>
-    <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
-      <c r="F10" s="9"/>
+    <row r="9" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="8">
+        <v>42838</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="8">
+        <v>42838</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="8"/>

</xml_diff>

<commit_message>
VLAB #33247  add I/O needed to invoke 2D_AR in the selectivity setup; keep version at 3.30.03.00
</commit_message>
<xml_diff>
--- a/SS_330_Change_Log.xlsx
+++ b/SS_330_Change_Log.xlsx
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="39">
   <si>
     <t>Date</t>
   </si>
@@ -165,7 +165,19 @@
     <t>add ability to have expected values in forecast; all data read after retroyr set to have no logL; also add explicit timing option (month&gt;1000) for fishery samples</t>
   </si>
   <si>
-    <t>04/13/2017 for 3.30.02.00</t>
+    <t>3.30.03.00</t>
+  </si>
+  <si>
+    <t>statistics</t>
+  </si>
+  <si>
+    <t>modify I/O in selectivity setup to invoke 2d_AR1 selectivity; but functional code still in development</t>
+  </si>
+  <si>
+    <t>modify I/O in survey CPUE setup for getting sdreport on survey expected value; but functional code still in development</t>
+  </si>
+  <si>
+    <t>04/18/2017 for 3.30.03.00</t>
   </si>
 </sst>
 </file>
@@ -601,7 +613,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
+      <selection pane="bottomLeft" activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -623,7 +635,7 @@
         <v>8</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25"/>
@@ -767,13 +779,39 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
-      <c r="F11" s="9"/>
+    <row r="11" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A11" s="8">
+        <v>42839</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="8"/>
-      <c r="F12" s="9"/>
+      <c r="A12" s="8">
+        <v>42843</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="8"/>

</xml_diff>

<commit_message>
update SS_330_change_Log.xlsx thru 3.30.03.04
</commit_message>
<xml_diff>
--- a/SS_330_Change_Log.xlsx
+++ b/SS_330_Change_Log.xlsx
@@ -17,8 +17,8 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$3:$E$216</definedName>
-    <definedName name="_xlnm.database">Sheet1!$A$3:$F$101</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$3:$E$217</definedName>
+    <definedName name="_xlnm.database">Sheet1!$A$3:$F$102</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="53">
   <si>
     <t>Date</t>
   </si>
@@ -177,7 +177,49 @@
     <t>modify I/O in survey CPUE setup for getting sdreport on survey expected value; but functional code still in development</t>
   </si>
   <si>
-    <t>04/18/2017 for 3.30.03.00</t>
+    <t>3.30.03.01</t>
+  </si>
+  <si>
+    <t>correct order of parameter reporting in parmtrace and posteriors; correct issue in autogenerate of dev se</t>
+  </si>
+  <si>
+    <t>3.30.03.02</t>
+  </si>
+  <si>
+    <t>3.30.03.03</t>
+  </si>
+  <si>
+    <t>3.30.03.04</t>
+  </si>
+  <si>
+    <t>growth</t>
+  </si>
+  <si>
+    <t>correct issue with Lorenzen M when growth is not estimated</t>
+  </si>
+  <si>
+    <t>fix doubled logL from forecast recruitments; investigate issue with blocks ending at endyr, not endyr+1</t>
+  </si>
+  <si>
+    <t>update</t>
+  </si>
+  <si>
+    <t>update sdreport for index values</t>
+  </si>
+  <si>
+    <t>major re-work of echoinput during reading of forecast.ss</t>
+  </si>
+  <si>
+    <t>report</t>
+  </si>
+  <si>
+    <t>spawn_recruit</t>
+  </si>
+  <si>
+    <t>correct reporting of mature biomass and mature numbers in forecast</t>
+  </si>
+  <si>
+    <t>05/10/2017 for 3.30.03.04</t>
   </si>
 </sst>
 </file>
@@ -187,7 +229,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -239,6 +281,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF333333"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -277,7 +325,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -304,6 +352,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -609,9 +658,9 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:F363"/>
+  <dimension ref="A1:F364"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="F1" sqref="F1"/>
     </sheetView>
@@ -635,7 +684,7 @@
         <v>8</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25"/>
@@ -813,40 +862,133 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="8"/>
-      <c r="F13" s="9"/>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="8">
+        <v>42843</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="14" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="8"/>
-      <c r="F14" s="9"/>
-    </row>
-    <row r="15" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="8"/>
-      <c r="F15" s="9"/>
-    </row>
-    <row r="16" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="8"/>
-      <c r="F16" s="9"/>
+      <c r="A14" s="8">
+        <v>42856</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="8">
+        <v>42863</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F15" s="14" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="8">
+        <v>42863</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="17" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="8"/>
-      <c r="F17" s="9"/>
+      <c r="A17" s="8">
+        <v>42865</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="18" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="8"/>
-      <c r="F18" s="9"/>
+      <c r="A18" s="8">
+        <v>42865</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="19" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="8"/>
+      <c r="B19" s="5" t="s">
+        <v>34</v>
+      </c>
       <c r="F19" s="9"/>
     </row>
     <row r="20" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="8"/>
+      <c r="B20" s="5" t="s">
+        <v>34</v>
+      </c>
       <c r="F20" s="9"/>
     </row>
     <row r="21" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="8"/>
+      <c r="B21" s="5" t="s">
+        <v>34</v>
+      </c>
       <c r="F21" s="9"/>
     </row>
     <row r="22" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -953,15 +1095,15 @@
       <c r="A47" s="8"/>
       <c r="F47" s="9"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="8"/>
+      <c r="F48" s="9"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="8"/>
     </row>
-    <row r="50" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="8"/>
-      <c r="F50" s="9"/>
     </row>
     <row r="51" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" s="8"/>
@@ -979,12 +1121,12 @@
       <c r="A54" s="8"/>
       <c r="F54" s="9"/>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" s="8"/>
-    </row>
-    <row r="56" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F55" s="9"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="8"/>
-      <c r="F56" s="9"/>
     </row>
     <row r="57" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" s="8"/>
@@ -998,15 +1140,15 @@
       <c r="A59" s="8"/>
       <c r="F59" s="9"/>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A60" s="8"/>
+      <c r="F60" s="9"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="8"/>
     </row>
-    <row r="62" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="8"/>
-      <c r="F62" s="9"/>
     </row>
     <row r="63" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A63" s="8"/>
@@ -1028,12 +1170,12 @@
       <c r="A67" s="8"/>
       <c r="F67" s="9"/>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A68" s="8"/>
-    </row>
-    <row r="69" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F68" s="9"/>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="8"/>
-      <c r="F69" s="9"/>
     </row>
     <row r="70" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A70" s="8"/>
@@ -1059,19 +1201,20 @@
       <c r="A75" s="8"/>
       <c r="F75" s="9"/>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A76" s="8"/>
-    </row>
-    <row r="77" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F76" s="9"/>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="8"/>
-      <c r="F77" s="9"/>
     </row>
     <row r="78" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A78" s="8"/>
       <c r="F78" s="9"/>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A79" s="8"/>
+      <c r="F79" s="9"/>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="8"/>
@@ -1147,10 +1290,10 @@
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" s="8"/>
-      <c r="F104" s="3"/>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" s="8"/>
+      <c r="F105" s="3"/>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" s="8"/>
@@ -1175,7 +1318,6 @@
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" s="8"/>
-      <c r="F113" s="3"/>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" s="8"/>
@@ -1183,7 +1325,6 @@
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" s="8"/>
-      <c r="B115"/>
       <c r="F115" s="3"/>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
@@ -1209,7 +1350,6 @@
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" s="8"/>
       <c r="B120"/>
-      <c r="C120"/>
       <c r="F120" s="3"/>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
@@ -1228,14 +1368,14 @@
       <c r="A123" s="8"/>
       <c r="B123"/>
       <c r="C123"/>
-      <c r="D123"/>
-      <c r="E123"/>
       <c r="F123" s="3"/>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" s="8"/>
       <c r="B124"/>
       <c r="C124"/>
+      <c r="D124"/>
+      <c r="E124"/>
       <c r="F124" s="3"/>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
@@ -1376,13 +1516,13 @@
       <c r="C147"/>
       <c r="F147" s="3"/>
     </row>
-    <row r="148" spans="1:6" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A148" s="8"/>
       <c r="B148"/>
       <c r="C148"/>
       <c r="F148" s="3"/>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:6" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" s="8"/>
       <c r="B149"/>
       <c r="C149"/>
@@ -1400,13 +1540,13 @@
       <c r="C151"/>
       <c r="F151" s="3"/>
     </row>
-    <row r="152" spans="1:6" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A152" s="8"/>
       <c r="B152"/>
       <c r="C152"/>
       <c r="F152" s="3"/>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:6" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" s="8"/>
       <c r="B153"/>
       <c r="C153"/>
@@ -1732,6 +1872,9 @@
     </row>
     <row r="207" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A207" s="8"/>
+      <c r="B207"/>
+      <c r="C207"/>
+      <c r="F207" s="3"/>
     </row>
     <row r="208" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A208" s="8"/>
@@ -1755,30 +1898,30 @@
       <c r="A214" s="8"/>
     </row>
     <row r="215" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A215" s="13"/>
+      <c r="A215" s="8"/>
     </row>
     <row r="216" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A216" s="10" t="s">
+      <c r="A216" s="13"/>
+    </row>
+    <row r="217" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A217" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B216" s="11" t="s">
+      <c r="B217" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C216" s="11" t="s">
+      <c r="C217" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D216" s="11" t="s">
+      <c r="D217" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E216" s="11" t="s">
+      <c r="E217" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="F216" s="12" t="s">
+      <c r="F217" s="12" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="217" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A217" s="8"/>
     </row>
     <row r="218" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A218" s="8"/>
@@ -2218,8 +2361,11 @@
     <row r="363" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A363" s="8"/>
     </row>
+    <row r="364" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A364" s="8"/>
+    </row>
   </sheetData>
-  <autoFilter ref="B3:E216"/>
+  <autoFilter ref="B3:E217"/>
   <sortState ref="A4:G99">
     <sortCondition ref="A4:A99"/>
     <sortCondition ref="B4:B99"/>

</xml_diff>

<commit_message>
VLAB #34515  convert birthseasons to settlement events
</commit_message>
<xml_diff>
--- a/SS_330_Change_Log.xlsx
+++ b/SS_330_Change_Log.xlsx
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="55">
   <si>
     <t>Date</t>
   </si>
@@ -219,7 +219,13 @@
     <t>correct reporting of mature biomass and mature numbers in forecast</t>
   </si>
   <si>
-    <t>05/10/2017 for 3.30.03.04</t>
+    <t>05/23/2017 for 3.30.04.01</t>
+  </si>
+  <si>
+    <t>3.30.04.01</t>
+  </si>
+  <si>
+    <t>convert conversion of 3.24's birthseason to 3.30's settlement events and revise required number of recruitment distribution parameters</t>
   </si>
 </sst>
 </file>
@@ -660,9 +666,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:F364"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="F1" sqref="F1"/>
+      <selection pane="bottomLeft" activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -970,12 +976,25 @@
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="8"/>
+    <row r="19" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A19" s="8">
+        <v>42878</v>
+      </c>
       <c r="B19" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="F19" s="9"/>
+        <v>53</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="20" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="8"/>

</xml_diff>

<commit_message>
keep version #; fix index issue with Qparm in trans; fix output issue for tag-recapture random data
</commit_message>
<xml_diff>
--- a/SS_330_Change_Log.xlsx
+++ b/SS_330_Change_Log.xlsx
@@ -20,7 +20,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$3:$E$217</definedName>
     <definedName name="_xlnm.database">Sheet1!$A$3:$F$102</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="57">
   <si>
     <t>Date</t>
   </si>
@@ -226,6 +226,12 @@
   </si>
   <si>
     <t>convert conversion of 3.24's birthseason to 3.30's settlement events and revise required number of recruitment distribution parameters</t>
+  </si>
+  <si>
+    <t>various</t>
+  </si>
+  <si>
+    <t>fix index issue in converter for MGparm seasonal effects and for retention if fleet &gt;1; fix hermaphrodites in forecast</t>
   </si>
 </sst>
 </file>
@@ -668,7 +674,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="F23" sqref="F23"/>
+      <selection pane="bottomLeft" activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -996,12 +1002,22 @@
         <v>54</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="8"/>
+    <row r="20" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A20" s="8">
+        <v>42885</v>
+      </c>
       <c r="B20" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="F20" s="9"/>
+        <v>53</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="21" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="8"/>

</xml_diff>

<commit_message>
VLAB#35646  trap for bad settlement timings; and improve consistency of recruitment output in time_series
</commit_message>
<xml_diff>
--- a/SS_330_Change_Log.xlsx
+++ b/SS_330_Change_Log.xlsx
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="61">
   <si>
     <t>Date</t>
   </si>
@@ -219,9 +219,6 @@
     <t>correct reporting of mature biomass and mature numbers in forecast</t>
   </si>
   <si>
-    <t>05/23/2017 for 3.30.04.01</t>
-  </si>
-  <si>
     <t>3.30.04.01</t>
   </si>
   <si>
@@ -232,6 +229,21 @@
   </si>
   <si>
     <t>fix index issue in converter for MGparm seasonal effects and for retention if fleet &gt;1; fix hermaphrodites in forecast</t>
+  </si>
+  <si>
+    <t>3.30.05.01</t>
+  </si>
+  <si>
+    <t>3.30.05.02</t>
+  </si>
+  <si>
+    <t>min sample size now is input; also placeholder input in forecast.ss for selectivity method</t>
+  </si>
+  <si>
+    <t>fix issue with settlement events happening in same season as birth_season</t>
+  </si>
+  <si>
+    <t>06/283/2017 for 3.30.05.02</t>
   </si>
 </sst>
 </file>
@@ -674,7 +686,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="F20" sqref="F20"/>
+      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -696,7 +708,7 @@
         <v>8</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25"/>
@@ -987,7 +999,7 @@
         <v>42878</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>24</v>
@@ -999,7 +1011,7 @@
         <v>50</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
@@ -1007,28 +1019,51 @@
         <v>42885</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D20" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="F20" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="F20" s="9" t="s">
+    </row>
+    <row r="21" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="8">
+        <v>42907</v>
+      </c>
+      <c r="B21" s="5" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="8"/>
-      <c r="B21" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="F21" s="9"/>
+      <c r="C21" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="22" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="8"/>
-      <c r="F22" s="9"/>
+      <c r="A22" s="8">
+        <v>42914</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="23" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="8"/>

</xml_diff>

<commit_message>
update version log to 3.30.06.01
</commit_message>
<xml_diff>
--- a/SS_330_Change_Log.xlsx
+++ b/SS_330_Change_Log.xlsx
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="64">
   <si>
     <t>Date</t>
   </si>
@@ -243,7 +243,16 @@
     <t>fix issue with settlement events happening in same season as birth_season</t>
   </si>
   <si>
-    <t>06/283/2017 for 3.30.05.02</t>
+    <t>3.30.06.01</t>
+  </si>
+  <si>
+    <t>survey</t>
+  </si>
+  <si>
+    <t>enhance control of phases when using depletion fleet; no mandatory I/O change</t>
+  </si>
+  <si>
+    <t>07/12/2017 for 3.30.06.01</t>
   </si>
 </sst>
 </file>
@@ -686,7 +695,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
+      <selection pane="bottomLeft" activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -708,7 +717,7 @@
         <v>8</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25"/>
@@ -1066,8 +1075,21 @@
       </c>
     </row>
     <row r="23" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="8"/>
-      <c r="F23" s="9"/>
+      <c r="A23" s="8">
+        <v>42928</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="24" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="8"/>

</xml_diff>

<commit_message>
VLAB #36450  fix forecast selectivity  3.30.06.02
</commit_message>
<xml_diff>
--- a/SS_330_Change_Log.xlsx
+++ b/SS_330_Change_Log.xlsx
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="73">
   <si>
     <t>Date</t>
   </si>
@@ -252,7 +252,34 @@
     <t>enhance control of phases when using depletion fleet; no mandatory I/O change</t>
   </si>
   <si>
-    <t>07/12/2017 for 3.30.06.01</t>
+    <t>07/26/2017 for 3.30.06.02</t>
+  </si>
+  <si>
+    <t>3.30.06.02</t>
+  </si>
+  <si>
+    <t>fix problem that overwrote averaged forecast selectivity with base selectivity when time-varying was used</t>
+  </si>
+  <si>
+    <t>improve reporting of selectivity in forecast era</t>
+  </si>
+  <si>
+    <t>agecomp</t>
+  </si>
+  <si>
+    <t>report more info in fit_age_comps section to match what is displayed for fit_len_comps</t>
+  </si>
+  <si>
+    <t>fix reporting of dev column in INDEX_2 section of report.sso</t>
+  </si>
+  <si>
+    <t>blocks</t>
+  </si>
+  <si>
+    <t>remove the constrant that the blocks cannot end after retroyr in order to allow changes in forecast</t>
+  </si>
+  <si>
+    <t>add column with ABC_buffer to time_series table in report.sso</t>
   </si>
 </sst>
 </file>
@@ -694,8 +721,8 @@
   <dimension ref="A1:F364"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="F1" sqref="F1"/>
+      <pane ySplit="3" topLeftCell="A11" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1091,29 +1118,119 @@
         <v>62</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="8"/>
-      <c r="F24" s="9"/>
+    <row r="24" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A24" s="8">
+        <v>42942</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="25" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="8"/>
-      <c r="F25" s="9"/>
+      <c r="A25" s="8">
+        <v>42942</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F25" s="9" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="26" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="8"/>
-      <c r="F26" s="9"/>
+      <c r="A26" s="8">
+        <v>42942</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F26" s="9" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="27" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="8"/>
-      <c r="F27" s="9"/>
+      <c r="A27" s="8">
+        <v>42942</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F27" s="9" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="28" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="8"/>
-      <c r="F28" s="9"/>
+      <c r="A28" s="8">
+        <v>42942</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="F28" s="9" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="29" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="8"/>
-      <c r="F29" s="9"/>
+      <c r="A29" s="8">
+        <v>42942</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F29" s="9" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="30" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="8"/>

</xml_diff>

<commit_message>
VLAB #36815  VLAB #36814 VLAB #36813
</commit_message>
<xml_diff>
--- a/SS_330_Change_Log.xlsx
+++ b/SS_330_Change_Log.xlsx
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="81">
   <si>
     <t>Date</t>
   </si>
@@ -246,9 +246,6 @@
     <t>enhance control of phases when using depletion fleet; no mandatory I/O change</t>
   </si>
   <si>
-    <t>07/26/2017 for 3.30.06.02</t>
-  </si>
-  <si>
     <t>3.30.06.02</t>
   </si>
   <si>
@@ -286,6 +283,27 @@
   </si>
   <si>
     <t>fix recruitment reporting issue when settlement events happen in same season as spawn_season</t>
+  </si>
+  <si>
+    <t>08/07/2017 for 3.30.07.01</t>
+  </si>
+  <si>
+    <t>3.30.07.01</t>
+  </si>
+  <si>
+    <t>benchmark</t>
+  </si>
+  <si>
+    <t>augmentation of SPR/YPR profile to show mean age of catch and other updates</t>
+  </si>
+  <si>
+    <t>fishing mortality</t>
+  </si>
+  <si>
+    <t>input</t>
+  </si>
+  <si>
+    <t>revise detailed F input to allow filling all years with one input record</t>
   </si>
 </sst>
 </file>
@@ -728,7 +746,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A17" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="F27" sqref="F27"/>
+      <selection pane="bottomLeft" activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -750,7 +768,7 @@
         <v>8</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>61</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25"/>
@@ -1087,7 +1105,7 @@
         <v>54</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -1104,7 +1122,7 @@
         <v>54</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -1129,7 +1147,7 @@
         <v>42942</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>12</v>
@@ -1138,7 +1156,7 @@
         <v>13</v>
       </c>
       <c r="F24" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -1146,7 +1164,7 @@
         <v>42942</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>31</v>
@@ -1155,7 +1173,7 @@
         <v>25</v>
       </c>
       <c r="F25" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -1163,19 +1181,19 @@
         <v>42942</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>31</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E26" s="5" t="s">
         <v>49</v>
       </c>
       <c r="F26" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -1183,7 +1201,7 @@
         <v>42942</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>12</v>
@@ -1195,7 +1213,7 @@
         <v>49</v>
       </c>
       <c r="F27" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -1203,7 +1221,7 @@
         <v>42942</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>46</v>
@@ -1212,10 +1230,10 @@
         <v>25</v>
       </c>
       <c r="E28" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="F28" s="9" t="s">
         <v>67</v>
-      </c>
-      <c r="F28" s="9" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -1223,7 +1241,7 @@
         <v>42942</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>31</v>
@@ -1235,7 +1253,7 @@
         <v>49</v>
       </c>
       <c r="F29" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
@@ -1243,25 +1261,57 @@
         <v>42943</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D30" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="F30" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="F30" s="9" t="s">
-        <v>71</v>
-      </c>
     </row>
     <row r="31" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="8"/>
-      <c r="F31" s="9"/>
+      <c r="A31" s="8">
+        <v>42954</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F31" s="9" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="32" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="8"/>
-      <c r="F32" s="9"/>
+      <c r="A32" s="8">
+        <v>42954</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="F32" s="9" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="33" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="8"/>

</xml_diff>

<commit_message>
VLAB #37058  fix age-specific K and growth with advanced settlement setups
</commit_message>
<xml_diff>
--- a/SS_330_Change_Log.xlsx
+++ b/SS_330_Change_Log.xlsx
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="83">
   <si>
     <t>Date</t>
   </si>
@@ -285,9 +285,6 @@
     <t>fix recruitment reporting issue when settlement events happen in same season as spawn_season</t>
   </si>
   <si>
-    <t>08/07/2017 for 3.30.07.01</t>
-  </si>
-  <si>
     <t>3.30.07.01</t>
   </si>
   <si>
@@ -304,6 +301,15 @@
   </si>
   <si>
     <t>revise detailed F input to allow filling all years with one input record</t>
+  </si>
+  <si>
+    <t>08/15/2017 for 3.30.07.02</t>
+  </si>
+  <si>
+    <t>3.30.07.02</t>
+  </si>
+  <si>
+    <t>repair age-specific K; fix growth problem if settlement age &gt;0</t>
   </si>
 </sst>
 </file>
@@ -746,7 +752,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A17" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="F33" sqref="F33"/>
+      <selection pane="bottomLeft" activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -768,7 +774,7 @@
         <v>8</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25"/>
@@ -1278,19 +1284,19 @@
         <v>42954</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E31" s="5" t="s">
         <v>49</v>
       </c>
       <c r="F31" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -1298,24 +1304,37 @@
         <v>42954</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D32" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="E32" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="E32" s="5" t="s">
+      <c r="F32" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="F32" s="9" t="s">
-        <v>80</v>
-      </c>
     </row>
     <row r="33" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="8"/>
-      <c r="F33" s="9"/>
+      <c r="A33" s="8">
+        <v>42954</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F33" s="9" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="34" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="8"/>

</xml_diff>

<commit_message>
update change log and version to 3.30.08.01 due to conditional I/O change in forecast
</commit_message>
<xml_diff>
--- a/SS_330_Change_Log.xlsx
+++ b/SS_330_Change_Log.xlsx
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="86">
   <si>
     <t>Date</t>
   </si>
@@ -303,13 +303,22 @@
     <t>revise detailed F input to allow filling all years with one input record</t>
   </si>
   <si>
-    <t>08/15/2017 for 3.30.07.02</t>
-  </si>
-  <si>
     <t>3.30.07.02</t>
   </si>
   <si>
     <t>repair age-specific K; fix growth problem if settlement age &gt;0</t>
+  </si>
+  <si>
+    <t>08/29/2017 for 3.30.07.03</t>
+  </si>
+  <si>
+    <t>3.30.07.03</t>
+  </si>
+  <si>
+    <t>fleets</t>
+  </si>
+  <si>
+    <t>fix code that still needed fishing fleets before survey fleets; however tag parameters still need fishing fleets first.  That will be addressed soon.</t>
   </si>
 </sst>
 </file>
@@ -752,7 +761,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A17" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="F29" sqref="F29"/>
+      <selection pane="bottomLeft" activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -774,7 +783,7 @@
         <v>8</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25"/>
@@ -1321,10 +1330,10 @@
     </row>
     <row r="33" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="8">
-        <v>42954</v>
+        <v>42962</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C33" s="5" t="s">
         <v>12</v>
@@ -1333,12 +1342,25 @@
         <v>43</v>
       </c>
       <c r="F33" s="9" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="8"/>
-      <c r="F34" s="9"/>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A34" s="8">
+        <v>42976</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="F34" s="9" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="35" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="8"/>

</xml_diff>

<commit_message>
display selectivity and catchability options in control.ss_new
</commit_message>
<xml_diff>
--- a/SS_330_Change_Log.xlsx
+++ b/SS_330_Change_Log.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="345" windowWidth="16875" windowHeight="8700"/>
+    <workbookView xWindow="240" yWindow="345" windowWidth="16875" windowHeight="7635"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -309,16 +309,22 @@
     <t>repair age-specific K; fix growth problem if settlement age &gt;0</t>
   </si>
   <si>
-    <t>08/29/2017 for 3.30.07.03</t>
-  </si>
-  <si>
-    <t>3.30.07.03</t>
-  </si>
-  <si>
     <t>fleets</t>
   </si>
   <si>
-    <t>fix code that still needed fishing fleets before survey fleets; however tag parameters still need fishing fleets first.  That will be addressed soon.</t>
+    <t>3.30.08.01</t>
+  </si>
+  <si>
+    <t>08/29/2017 for 3.30.08.01</t>
+  </si>
+  <si>
+    <t>fix code that still needed fishing fleets before survey fleets; however tag parameters still need fishing fleets first.  That will be addressed soon.
+This fix creates a conditional I/O change in forecast.ss:
+2 # basis for fcast catch tuning and for fcast catch caps and allocation  (2=deadbio; 3=retainbio; 5=deadnum; 6=retainnum)
+# Conditional input if relative F choice = 2
+# enter list of:  season,  fleet, relF; if used, terminate with season=-9999
+1 1 1
+-9999 0 0  # terminator for list of relF</t>
   </si>
 </sst>
 </file>
@@ -760,8 +766,8 @@
   <dimension ref="A1:F364"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A17" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="F34" sqref="F34"/>
+      <pane ySplit="3" topLeftCell="A26" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -783,7 +789,7 @@
         <v>8</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25"/>
@@ -1345,7 +1351,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="141.75" x14ac:dyDescent="0.25">
       <c r="A34" s="8">
         <v>42976</v>
       </c>
@@ -1356,7 +1362,7 @@
         <v>12</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F34" s="9" t="s">
         <v>85</v>

</xml_diff>

<commit_message>
3.30.08.02  minor fixes  VLAB #37862 and VLAB #37573
</commit_message>
<xml_diff>
--- a/SS_330_Change_Log.xlsx
+++ b/SS_330_Change_Log.xlsx
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="92">
   <si>
     <t>Date</t>
   </si>
@@ -313,9 +313,6 @@
   </si>
   <si>
     <t>3.30.08.01</t>
-  </si>
-  <si>
-    <t>08/29/2017 for 3.30.08.01</t>
   </si>
   <si>
     <t>fix code that still needed fishing fleets before survey fleets; however tag parameters still need fishing fleets first.  That will be addressed soon.
@@ -326,13 +323,35 @@
 1 1 1
 -9999 0 0  # terminator for list of relF</t>
   </si>
+  <si>
+    <t>3.30.08.02</t>
+  </si>
+  <si>
+    <t>rebuild</t>
+  </si>
+  <si>
+    <t>test and confirm that rebuilder output is correct;  it was not fully correct in version 3.30.04.02</t>
+  </si>
+  <si>
+    <t>data_generator</t>
+  </si>
+  <si>
+    <t>fix range of years output of environmental data in data.ss_new</t>
+  </si>
+  <si>
+    <t>add info on selectivity and catchability options to control.ss_new</t>
+  </si>
+  <si>
+    <t>2017-09-11  for 3.30.08.02</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
+    <numFmt numFmtId="167" formatCode="[$-10409]yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -430,7 +449,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -458,6 +477,7 @@
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -766,8 +786,8 @@
   <dimension ref="A1:F364"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A26" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="F32" sqref="F32"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="D116" sqref="D116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -789,7 +809,7 @@
         <v>8</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25"/>
@@ -823,7 +843,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="8">
+      <c r="A5" s="15">
         <v>42683</v>
       </c>
       <c r="B5" s="5" t="s">
@@ -840,7 +860,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="8">
+      <c r="A6" s="15">
         <v>42689</v>
       </c>
       <c r="B6" s="5" t="s">
@@ -860,7 +880,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="8">
+      <c r="A7" s="15">
         <v>42691</v>
       </c>
       <c r="B7" s="5" t="s">
@@ -880,7 +900,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="8">
+      <c r="A8" s="15">
         <v>42696</v>
       </c>
       <c r="B8" s="5" t="s">
@@ -900,7 +920,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="8">
+      <c r="A9" s="15">
         <v>42838</v>
       </c>
       <c r="B9" s="5" t="s">
@@ -914,7 +934,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="8">
+      <c r="A10" s="15">
         <v>42838</v>
       </c>
       <c r="B10" s="5" t="s">
@@ -934,7 +954,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="8">
+      <c r="A11" s="15">
         <v>42839</v>
       </c>
       <c r="B11" s="5" t="s">
@@ -951,7 +971,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="8">
+      <c r="A12" s="15">
         <v>42843</v>
       </c>
       <c r="B12" s="5" t="s">
@@ -968,7 +988,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="8">
+      <c r="A13" s="15">
         <v>42843</v>
       </c>
       <c r="B13" s="5" t="s">
@@ -985,7 +1005,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="8">
+      <c r="A14" s="15">
         <v>42856</v>
       </c>
       <c r="B14" s="5" t="s">
@@ -1002,7 +1022,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="8">
+      <c r="A15" s="15">
         <v>42863</v>
       </c>
       <c r="B15" s="5" t="s">
@@ -1019,7 +1039,7 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="8">
+      <c r="A16" s="15">
         <v>42863</v>
       </c>
       <c r="B16" s="5" t="s">
@@ -1036,7 +1056,7 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="8">
+      <c r="A17" s="15">
         <v>42865</v>
       </c>
       <c r="B17" s="5" t="s">
@@ -1056,7 +1076,7 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="8">
+      <c r="A18" s="15">
         <v>42865</v>
       </c>
       <c r="B18" s="5" t="s">
@@ -1076,7 +1096,7 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A19" s="8">
+      <c r="A19" s="15">
         <v>42878</v>
       </c>
       <c r="B19" s="5" t="s">
@@ -1096,7 +1116,7 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A20" s="8">
+      <c r="A20" s="15">
         <v>42885</v>
       </c>
       <c r="B20" s="5" t="s">
@@ -1113,7 +1133,7 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="8">
+      <c r="A21" s="15">
         <v>42907</v>
       </c>
       <c r="B21" s="5" t="s">
@@ -1130,7 +1150,7 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="8">
+      <c r="A22" s="15">
         <v>42914</v>
       </c>
       <c r="B22" s="5" t="s">
@@ -1147,7 +1167,7 @@
       </c>
     </row>
     <row r="23" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="8">
+      <c r="A23" s="15">
         <v>42928</v>
       </c>
       <c r="B23" s="5" t="s">
@@ -1164,7 +1184,7 @@
       </c>
     </row>
     <row r="24" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A24" s="8">
+      <c r="A24" s="15">
         <v>42942</v>
       </c>
       <c r="B24" s="5" t="s">
@@ -1181,7 +1201,7 @@
       </c>
     </row>
     <row r="25" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="8">
+      <c r="A25" s="15">
         <v>42942</v>
       </c>
       <c r="B25" s="5" t="s">
@@ -1198,7 +1218,7 @@
       </c>
     </row>
     <row r="26" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="8">
+      <c r="A26" s="15">
         <v>42942</v>
       </c>
       <c r="B26" s="5" t="s">
@@ -1218,7 +1238,7 @@
       </c>
     </row>
     <row r="27" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="8">
+      <c r="A27" s="15">
         <v>42942</v>
       </c>
       <c r="B27" s="5" t="s">
@@ -1238,7 +1258,7 @@
       </c>
     </row>
     <row r="28" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="8">
+      <c r="A28" s="15">
         <v>42942</v>
       </c>
       <c r="B28" s="5" t="s">
@@ -1258,7 +1278,7 @@
       </c>
     </row>
     <row r="29" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="8">
+      <c r="A29" s="15">
         <v>42942</v>
       </c>
       <c r="B29" s="5" t="s">
@@ -1278,7 +1298,7 @@
       </c>
     </row>
     <row r="30" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A30" s="8">
+      <c r="A30" s="15">
         <v>42943</v>
       </c>
       <c r="B30" s="5" t="s">
@@ -1295,7 +1315,7 @@
       </c>
     </row>
     <row r="31" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="8">
+      <c r="A31" s="15">
         <v>42954</v>
       </c>
       <c r="B31" s="5" t="s">
@@ -1315,7 +1335,7 @@
       </c>
     </row>
     <row r="32" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="8">
+      <c r="A32" s="15">
         <v>42954</v>
       </c>
       <c r="B32" s="5" t="s">
@@ -1335,7 +1355,7 @@
       </c>
     </row>
     <row r="33" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="8">
+      <c r="A33" s="15">
         <v>42962</v>
       </c>
       <c r="B33" s="5" t="s">
@@ -1352,7 +1372,7 @@
       </c>
     </row>
     <row r="34" spans="1:6" ht="141.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="8">
+      <c r="A34" s="15">
         <v>42976</v>
       </c>
       <c r="B34" s="5" t="s">
@@ -1365,338 +1385,377 @@
         <v>82</v>
       </c>
       <c r="F34" s="9" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="15">
+        <v>42989</v>
+      </c>
+      <c r="B35" s="5" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="8"/>
-      <c r="F35" s="9"/>
+      <c r="C35" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="F35" s="9" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="36" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="8"/>
-      <c r="F36" s="9"/>
+      <c r="A36" s="15">
+        <v>42989</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="F36" s="9" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="37" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="8"/>
-      <c r="F37" s="9"/>
+      <c r="A37" s="15">
+        <v>42989</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F37" s="9" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="38" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="8"/>
+      <c r="A38" s="15"/>
       <c r="F38" s="9"/>
     </row>
     <row r="39" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="8"/>
+      <c r="A39" s="15"/>
       <c r="F39" s="9"/>
     </row>
     <row r="40" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="8"/>
+      <c r="A40" s="15"/>
       <c r="F40" s="9"/>
     </row>
     <row r="41" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="8"/>
+      <c r="A41" s="15"/>
       <c r="F41" s="9"/>
     </row>
     <row r="42" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A42" s="8"/>
+      <c r="A42" s="15"/>
       <c r="F42" s="9"/>
     </row>
     <row r="43" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A43" s="8"/>
+      <c r="A43" s="15"/>
       <c r="F43" s="9"/>
     </row>
     <row r="44" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A44" s="8"/>
+      <c r="A44" s="15"/>
       <c r="F44" s="9"/>
     </row>
     <row r="45" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A45" s="8"/>
+      <c r="A45" s="15"/>
       <c r="F45" s="9"/>
     </row>
     <row r="46" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A46" s="8"/>
+      <c r="A46" s="15"/>
       <c r="F46" s="9"/>
     </row>
     <row r="47" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A47" s="8"/>
+      <c r="A47" s="15"/>
       <c r="F47" s="9"/>
     </row>
     <row r="48" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A48" s="8"/>
+      <c r="A48" s="15"/>
       <c r="F48" s="9"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="8"/>
+      <c r="A49" s="15"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="8"/>
+      <c r="A50" s="15"/>
     </row>
     <row r="51" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="8"/>
+      <c r="A51" s="15"/>
       <c r="F51" s="9"/>
     </row>
     <row r="52" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A52" s="8"/>
+      <c r="A52" s="15"/>
       <c r="F52" s="9"/>
     </row>
     <row r="53" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="8"/>
+      <c r="A53" s="15"/>
       <c r="F53" s="9"/>
     </row>
     <row r="54" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A54" s="8"/>
+      <c r="A54" s="15"/>
       <c r="F54" s="9"/>
     </row>
     <row r="55" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A55" s="8"/>
+      <c r="A55" s="15"/>
       <c r="F55" s="9"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="8"/>
+      <c r="A56" s="15"/>
     </row>
     <row r="57" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A57" s="8"/>
+      <c r="A57" s="15"/>
       <c r="F57" s="9"/>
     </row>
     <row r="58" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A58" s="8"/>
+      <c r="A58" s="15"/>
       <c r="F58" s="9"/>
     </row>
     <row r="59" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A59" s="8"/>
+      <c r="A59" s="15"/>
       <c r="F59" s="9"/>
     </row>
     <row r="60" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A60" s="8"/>
+      <c r="A60" s="15"/>
       <c r="F60" s="9"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="8"/>
+      <c r="A61" s="15"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="8"/>
+      <c r="A62" s="15"/>
     </row>
     <row r="63" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A63" s="8"/>
+      <c r="A63" s="15"/>
       <c r="F63" s="9"/>
     </row>
     <row r="64" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A64" s="8"/>
+      <c r="A64" s="15"/>
       <c r="F64" s="9"/>
     </row>
     <row r="65" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A65" s="8"/>
+      <c r="A65" s="15"/>
       <c r="F65" s="9"/>
     </row>
     <row r="66" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A66" s="8"/>
+      <c r="A66" s="15"/>
       <c r="F66" s="9"/>
     </row>
     <row r="67" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A67" s="8"/>
+      <c r="A67" s="15"/>
       <c r="F67" s="9"/>
     </row>
     <row r="68" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A68" s="8"/>
+      <c r="A68" s="15"/>
       <c r="F68" s="9"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="8"/>
+      <c r="A69" s="15"/>
     </row>
     <row r="70" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A70" s="8"/>
+      <c r="A70" s="15"/>
       <c r="F70" s="9"/>
     </row>
     <row r="71" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A71" s="8"/>
+      <c r="A71" s="15"/>
       <c r="F71" s="9"/>
     </row>
     <row r="72" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A72" s="8"/>
+      <c r="A72" s="15"/>
       <c r="F72" s="9"/>
     </row>
     <row r="73" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A73" s="8"/>
+      <c r="A73" s="15"/>
       <c r="F73" s="9"/>
     </row>
     <row r="74" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A74" s="8"/>
+      <c r="A74" s="15"/>
       <c r="F74" s="9"/>
     </row>
     <row r="75" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A75" s="8"/>
+      <c r="A75" s="15"/>
       <c r="F75" s="9"/>
     </row>
     <row r="76" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A76" s="8"/>
+      <c r="A76" s="15"/>
       <c r="F76" s="9"/>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77" s="8"/>
+      <c r="A77" s="15"/>
     </row>
     <row r="78" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A78" s="8"/>
+      <c r="A78" s="15"/>
       <c r="F78" s="9"/>
     </row>
     <row r="79" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A79" s="8"/>
+      <c r="A79" s="15"/>
       <c r="F79" s="9"/>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A80" s="8"/>
+      <c r="A80" s="15"/>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A81" s="8"/>
+      <c r="A81" s="15"/>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A82" s="8"/>
+      <c r="A82" s="15"/>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A83" s="8"/>
+      <c r="A83" s="15"/>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A84" s="8"/>
+      <c r="A84" s="15"/>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A85" s="8"/>
+      <c r="A85" s="15"/>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A86" s="8"/>
+      <c r="A86" s="15"/>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A87" s="8"/>
+      <c r="A87" s="15"/>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A88" s="8"/>
+      <c r="A88" s="15"/>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A89" s="8"/>
+      <c r="A89" s="15"/>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A90" s="8"/>
+      <c r="A90" s="15"/>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A91" s="8"/>
+      <c r="A91" s="15"/>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A92" s="8"/>
+      <c r="A92" s="15"/>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A93" s="8"/>
+      <c r="A93" s="15"/>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A94" s="8"/>
+      <c r="A94" s="15"/>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A95" s="8"/>
+      <c r="A95" s="15"/>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A96" s="8"/>
+      <c r="A96" s="15"/>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A97" s="8"/>
+      <c r="A97" s="15"/>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A98" s="8"/>
+      <c r="A98" s="15"/>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A99" s="8"/>
+      <c r="A99" s="15"/>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A100" s="8"/>
+      <c r="A100" s="15"/>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A101" s="8"/>
+      <c r="A101" s="15"/>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A102" s="8"/>
+      <c r="A102" s="15"/>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A103" s="8"/>
+      <c r="A103" s="15"/>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A104" s="8"/>
+      <c r="A104" s="15"/>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A105" s="8"/>
+      <c r="A105" s="15"/>
       <c r="F105" s="3"/>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A106" s="8"/>
+      <c r="A106" s="15"/>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A107" s="8"/>
+      <c r="A107" s="15"/>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A108" s="8"/>
+      <c r="A108" s="15"/>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A109" s="8"/>
+      <c r="A109" s="15"/>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A110" s="8"/>
+      <c r="A110" s="15"/>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A111" s="8"/>
+      <c r="A111" s="15"/>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A112" s="8"/>
+      <c r="A112" s="15"/>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A113" s="8"/>
+      <c r="A113" s="15"/>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A114" s="8"/>
+      <c r="A114" s="15"/>
       <c r="F114" s="3"/>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A115" s="8"/>
+      <c r="A115" s="15"/>
       <c r="F115" s="3"/>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A116" s="8"/>
+      <c r="A116" s="15"/>
       <c r="B116"/>
       <c r="F116" s="3"/>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A117" s="8"/>
+      <c r="A117" s="15"/>
       <c r="B117"/>
       <c r="F117" s="3"/>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A118" s="8"/>
+      <c r="A118" s="15"/>
       <c r="B118"/>
       <c r="F118" s="3"/>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A119" s="8"/>
+      <c r="A119" s="15"/>
       <c r="B119"/>
       <c r="F119" s="3"/>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A120" s="8"/>
+      <c r="A120" s="15"/>
       <c r="B120"/>
       <c r="F120" s="3"/>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A121" s="8"/>
+      <c r="A121" s="15"/>
       <c r="B121"/>
       <c r="C121"/>
       <c r="F121" s="3"/>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A122" s="8"/>
+      <c r="A122" s="15"/>
       <c r="B122"/>
       <c r="C122"/>
       <c r="F122" s="3"/>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A123" s="8"/>
+      <c r="A123" s="15"/>
       <c r="B123"/>
       <c r="C123"/>
       <c r="F123" s="3"/>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A124" s="8"/>
+      <c r="A124" s="15"/>
       <c r="B124"/>
       <c r="C124"/>
       <c r="D124"/>
@@ -1704,7 +1763,7 @@
       <c r="F124" s="3"/>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A125" s="8"/>
+      <c r="A125" s="15"/>
       <c r="B125"/>
       <c r="C125"/>
       <c r="F125" s="3"/>

</xml_diff>

<commit_message>
final clean-up for 3.30.08.02
</commit_message>
<xml_diff>
--- a/SS_330_Change_Log.xlsx
+++ b/SS_330_Change_Log.xlsx
@@ -315,34 +315,33 @@
     <t>3.30.08.01</t>
   </si>
   <si>
+    <t>3.30.08.02</t>
+  </si>
+  <si>
+    <t>rebuild</t>
+  </si>
+  <si>
+    <t>test and confirm that rebuilder output is correct;  it was not fully correct in version 3.30.04.02</t>
+  </si>
+  <si>
+    <t>data_generator</t>
+  </si>
+  <si>
+    <t>fix range of years output of environmental data in data.ss_new</t>
+  </si>
+  <si>
+    <t>add info on selectivity and catchability options to control.ss_new</t>
+  </si>
+  <si>
+    <t>2017-09-11  for 3.30.08.02</t>
+  </si>
+  <si>
     <t>fix code that still needed fishing fleets before survey fleets; however tag parameters still need fishing fleets first.  That will be addressed soon.
 This fix creates a conditional I/O change in forecast.ss:
-2 # basis for fcast catch tuning and for fcast catch caps and allocation  (2=deadbio; 3=retainbio; 5=deadnum; 6=retainnum)
 # Conditional input if relative F choice = 2
 # enter list of:  season,  fleet, relF; if used, terminate with season=-9999
 1 1 1
 -9999 0 0  # terminator for list of relF</t>
-  </si>
-  <si>
-    <t>3.30.08.02</t>
-  </si>
-  <si>
-    <t>rebuild</t>
-  </si>
-  <si>
-    <t>test and confirm that rebuilder output is correct;  it was not fully correct in version 3.30.04.02</t>
-  </si>
-  <si>
-    <t>data_generator</t>
-  </si>
-  <si>
-    <t>fix range of years output of environmental data in data.ss_new</t>
-  </si>
-  <si>
-    <t>add info on selectivity and catchability options to control.ss_new</t>
-  </si>
-  <si>
-    <t>2017-09-11  for 3.30.08.02</t>
   </si>
 </sst>
 </file>
@@ -351,7 +350,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
-    <numFmt numFmtId="167" formatCode="[$-10409]yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="165" formatCode="[$-10409]yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -477,7 +476,7 @@
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -786,8 +785,8 @@
   <dimension ref="A1:F364"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="D116" sqref="D116"/>
+      <pane ySplit="3" topLeftCell="A25" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -809,7 +808,7 @@
         <v>8</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25"/>
@@ -1371,7 +1370,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="141.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A34" s="15">
         <v>42976</v>
       </c>
@@ -1385,7 +1384,7 @@
         <v>82</v>
       </c>
       <c r="F34" s="9" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -1393,16 +1392,16 @@
         <v>42989</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C35" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D35" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="F35" s="9" t="s">
         <v>86</v>
-      </c>
-      <c r="F35" s="9" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -1410,16 +1409,16 @@
         <v>42989</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C36" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D36" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="F36" s="9" t="s">
         <v>88</v>
-      </c>
-      <c r="F36" s="9" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -1427,7 +1426,7 @@
         <v>42989</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>31</v>
@@ -1436,7 +1435,7 @@
         <v>25</v>
       </c>
       <c r="F37" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
VLAB #38436  fix error in writing to ss_summary.sso
</commit_message>
<xml_diff>
--- a/SS_330_Change_Log.xlsx
+++ b/SS_330_Change_Log.xlsx
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="103">
   <si>
     <t>Date</t>
   </si>
@@ -331,9 +331,6 @@
   </si>
   <si>
     <t>add info on selectivity and catchability options to control.ss_new</t>
-  </si>
-  <si>
-    <t>2017-09-11  for 3.30.08.02</t>
   </si>
   <si>
     <t>fix code that still needed fishing fleets before survey fleets; however tag parameters still need fishing fleets first.  That will be addressed soon.
@@ -342,6 +339,42 @@
 # enter list of:  season,  fleet, relF; if used, terminate with season=-9999
 1 1 1
 -9999 0 0  # terminator for list of relF</t>
+  </si>
+  <si>
+    <t>I/O_Change</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Yes,  conditional in control file</t>
+  </si>
+  <si>
+    <t>Yes,  conditional in data file</t>
+  </si>
+  <si>
+    <t>Yes, mandatory in data file</t>
+  </si>
+  <si>
+    <t>Yes, mandatory in control file</t>
+  </si>
+  <si>
+    <t>Yes, mandatory in forecast file</t>
+  </si>
+  <si>
+    <t>3.30.08.03</t>
+  </si>
+  <si>
+    <t>putput</t>
+  </si>
+  <si>
+    <t>fix sometimes fatal error in writing to the new summary output file:  ss_summary.sso</t>
+  </si>
+  <si>
+    <t>2017-09-29 for 3.30.08.03</t>
   </si>
 </sst>
 </file>
@@ -448,7 +481,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -477,6 +510,7 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -782,11 +816,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:F364"/>
+  <dimension ref="A1:G364"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A25" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="F34" sqref="F34"/>
+      <pane ySplit="3" topLeftCell="A13" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -800,7 +834,7 @@
     <col min="7" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -808,11 +842,11 @@
         <v>8</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -831,8 +865,11 @@
       <c r="F3" s="7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G3" s="16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="8"/>
       <c r="B4" s="5" t="s">
         <v>9</v>
@@ -840,8 +877,11 @@
       <c r="F4" s="9" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G4" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="15">
         <v>42683</v>
       </c>
@@ -857,8 +897,11 @@
       <c r="F5" s="9" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G5" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="15">
         <v>42689</v>
       </c>
@@ -877,8 +920,11 @@
       <c r="F6" s="9" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G6" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="15">
         <v>42691</v>
       </c>
@@ -897,8 +943,11 @@
       <c r="F7" s="9" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="G7" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A8" s="15">
         <v>42696</v>
       </c>
@@ -917,8 +966,11 @@
       <c r="F8" s="9" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="G8" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A9" s="15">
         <v>42838</v>
       </c>
@@ -931,8 +983,11 @@
       <c r="F9" s="9" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="G9" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A10" s="15">
         <v>42838</v>
       </c>
@@ -951,8 +1006,11 @@
       <c r="F10" s="9" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="G10" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A11" s="15">
         <v>42839</v>
       </c>
@@ -968,8 +1026,11 @@
       <c r="F11" s="9" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G11" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="15">
         <v>42843</v>
       </c>
@@ -985,8 +1046,11 @@
       <c r="F12" s="9" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G12" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="15">
         <v>42843</v>
       </c>
@@ -1002,8 +1066,11 @@
       <c r="F13" s="14" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G13" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="15">
         <v>42856</v>
       </c>
@@ -1019,8 +1086,11 @@
       <c r="F14" s="9" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G14" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="15">
         <v>42863</v>
       </c>
@@ -1036,8 +1106,11 @@
       <c r="F15" s="14" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G15" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="15">
         <v>42863</v>
       </c>
@@ -1053,8 +1126,11 @@
       <c r="F16" s="14" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G16" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="15">
         <v>42865</v>
       </c>
@@ -1073,8 +1149,11 @@
       <c r="F17" s="9" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G17" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="15">
         <v>42865</v>
       </c>
@@ -1093,8 +1172,11 @@
       <c r="F18" s="9" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="G18" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A19" s="15">
         <v>42878</v>
       </c>
@@ -1113,8 +1195,11 @@
       <c r="F19" s="9" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="G19" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A20" s="15">
         <v>42885</v>
       </c>
@@ -1130,8 +1215,11 @@
       <c r="F20" s="9" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G20" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="15">
         <v>42907</v>
       </c>
@@ -1147,8 +1235,11 @@
       <c r="F21" s="9" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G21" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="15">
         <v>42914</v>
       </c>
@@ -1164,8 +1255,11 @@
       <c r="F22" s="9" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G22" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="15">
         <v>42928</v>
       </c>
@@ -1181,8 +1275,11 @@
       <c r="F23" s="9" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="G23" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A24" s="15">
         <v>42942</v>
       </c>
@@ -1198,8 +1295,11 @@
       <c r="F24" s="9" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G24" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="15">
         <v>42942</v>
       </c>
@@ -1215,8 +1315,11 @@
       <c r="F25" s="9" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G25" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="15">
         <v>42942</v>
       </c>
@@ -1235,8 +1338,11 @@
       <c r="F26" s="9" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G26" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="15">
         <v>42942</v>
       </c>
@@ -1255,8 +1361,11 @@
       <c r="F27" s="9" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G27" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="15">
         <v>42942</v>
       </c>
@@ -1275,8 +1384,11 @@
       <c r="F28" s="9" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G28" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="15">
         <v>42942</v>
       </c>
@@ -1295,8 +1407,11 @@
       <c r="F29" s="9" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="G29" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A30" s="15">
         <v>42943</v>
       </c>
@@ -1312,8 +1427,11 @@
       <c r="F30" s="9" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G30" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="15">
         <v>42954</v>
       </c>
@@ -1332,8 +1450,11 @@
       <c r="F31" s="9" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G31" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="15">
         <v>42954</v>
       </c>
@@ -1352,8 +1473,11 @@
       <c r="F32" s="9" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G32" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="15">
         <v>42962</v>
       </c>
@@ -1369,8 +1493,11 @@
       <c r="F33" s="9" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="G33" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A34" s="15">
         <v>42976</v>
       </c>
@@ -1384,10 +1511,13 @@
         <v>82</v>
       </c>
       <c r="F34" s="9" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+      <c r="G34" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="15">
         <v>42989</v>
       </c>
@@ -1403,8 +1533,11 @@
       <c r="F35" s="9" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G35" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="15">
         <v>42989</v>
       </c>
@@ -1420,8 +1553,11 @@
       <c r="F36" s="9" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G36" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="15">
         <v>42989</v>
       </c>
@@ -1437,48 +1573,67 @@
       <c r="F37" s="9" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="15"/>
-      <c r="F38" s="9"/>
-    </row>
-    <row r="39" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G37" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="15">
+        <v>43007</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="F38" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="G38" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="15"/>
       <c r="F39" s="9"/>
     </row>
-    <row r="40" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="15"/>
       <c r="F40" s="9"/>
     </row>
-    <row r="41" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="15"/>
       <c r="F41" s="9"/>
     </row>
-    <row r="42" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="15"/>
       <c r="F42" s="9"/>
     </row>
-    <row r="43" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="15"/>
       <c r="F43" s="9"/>
     </row>
-    <row r="44" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="15"/>
       <c r="F44" s="9"/>
     </row>
-    <row r="45" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="15"/>
       <c r="F45" s="9"/>
     </row>
-    <row r="46" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="15"/>
       <c r="F46" s="9"/>
     </row>
-    <row r="47" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="15"/>
       <c r="F47" s="9"/>
     </row>
-    <row r="48" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="15"/>
       <c r="F48" s="9"/>
     </row>

</xml_diff>

<commit_message>
VLAB #40546  fix error in forecast recr when spawn_month>1
</commit_message>
<xml_diff>
--- a/SS_330_Change_Log.xlsx
+++ b/SS_330_Change_Log.xlsx
@@ -368,13 +368,13 @@
     <t>3.30.08.03</t>
   </si>
   <si>
-    <t>putput</t>
-  </si>
-  <si>
     <t>fix sometimes fatal error in writing to the new summary output file:  ss_summary.sso</t>
   </si>
   <si>
     <t>2017-09-29 for 3.30.08.03</t>
+  </si>
+  <si>
+    <t>output</t>
   </si>
 </sst>
 </file>
@@ -819,8 +819,8 @@
   <dimension ref="A1:G364"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A13" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="F31" sqref="F31"/>
+      <pane ySplit="3" topLeftCell="A28" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -842,7 +842,7 @@
         <v>8</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25"/>
@@ -1588,10 +1588,10 @@
         <v>31</v>
       </c>
       <c r="D38" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="F38" s="9" t="s">
         <v>100</v>
-      </c>
-      <c r="F38" s="9" t="s">
-        <v>101</v>
       </c>
       <c r="G38" s="5" t="s">
         <v>93</v>

</xml_diff>

<commit_message>
update change log for 3.30.08.04
</commit_message>
<xml_diff>
--- a/SS_330_Change_Log.xlsx
+++ b/SS_330_Change_Log.xlsx
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="105">
   <si>
     <t>Date</t>
   </si>
@@ -371,10 +371,16 @@
     <t>fix sometimes fatal error in writing to the new summary output file:  ss_summary.sso</t>
   </si>
   <si>
-    <t>2017-09-29 for 3.30.08.03</t>
-  </si>
-  <si>
     <t>output</t>
+  </si>
+  <si>
+    <t>3.30.08.04</t>
+  </si>
+  <si>
+    <t>fix forecast recruitment error when spawn_month&gt;1</t>
+  </si>
+  <si>
+    <t>2017-11-06 for 3.30.08.04</t>
   </si>
 </sst>
 </file>
@@ -820,7 +826,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A28" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="F41" sqref="F41"/>
+      <selection pane="bottomLeft" activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -842,7 +848,7 @@
         <v>8</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25"/>
@@ -1588,7 +1594,7 @@
         <v>31</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F38" s="9" t="s">
         <v>100</v>
@@ -1598,8 +1604,24 @@
       </c>
     </row>
     <row r="39" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="15"/>
-      <c r="F39" s="9"/>
+      <c r="A39" s="15">
+        <v>43045</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F39" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="G39" s="5" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="40" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="15"/>

</xml_diff>

<commit_message>
clean-up some warning messages; enable long forecasts; limit biasadj in forecast
</commit_message>
<xml_diff>
--- a/SS_330_Change_Log.xlsx
+++ b/SS_330_Change_Log.xlsx
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="107">
   <si>
     <t>Date</t>
   </si>
@@ -380,7 +380,13 @@
     <t>fix forecast recruitment error when spawn_month&gt;1</t>
   </si>
   <si>
-    <t>2017-11-06 for 3.30.08.04</t>
+    <t>after biasadjustment ramp is calculated, set biasadjustment to 0.0 for years after recdev_end</t>
+  </si>
+  <si>
+    <t>2017-11-07 for 3.30.08.04</t>
+  </si>
+  <si>
+    <t>improve some warnings and adjust array dimensions to allow very long forecasts</t>
   </si>
 </sst>
 </file>
@@ -826,7 +832,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A28" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="F33" sqref="F33"/>
+      <selection pane="bottomLeft" activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -848,7 +854,7 @@
         <v>8</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25"/>
@@ -1591,7 +1597,7 @@
         <v>99</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="D38" s="5" t="s">
         <v>101</v>
@@ -1611,7 +1617,7 @@
         <v>102</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="D39" s="5" t="s">
         <v>13</v>
@@ -1624,12 +1630,44 @@
       </c>
     </row>
     <row r="40" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="15"/>
-      <c r="F40" s="9"/>
+      <c r="A40" s="15">
+        <v>43046</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="F40" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="G40" s="5" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="41" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="15"/>
-      <c r="F41" s="9"/>
+      <c r="A41" s="15">
+        <v>43046</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="F41" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="G41" s="5" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="42" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="15"/>

</xml_diff>

<commit_message>
VLAB #41140.  Add controls for forecast recruitment
</commit_message>
<xml_diff>
--- a/SS_330_Change_Log.xlsx
+++ b/SS_330_Change_Log.xlsx
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="110">
   <si>
     <t>Date</t>
   </si>
@@ -383,10 +383,19 @@
     <t>after biasadjustment ramp is calculated, set biasadjustment to 0.0 for years after recdev_end</t>
   </si>
   <si>
-    <t>2017-11-07 for 3.30.08.04</t>
-  </si>
-  <si>
     <t>improve some warnings and adjust array dimensions to allow very long forecasts</t>
+  </si>
+  <si>
+    <t>2017-11-20 for 3.30.09.00</t>
+  </si>
+  <si>
+    <t>3.30.09.00</t>
+  </si>
+  <si>
+    <t>provide controls for extrapolating 2D_AR selectivity outside of year range of the devs</t>
+  </si>
+  <si>
+    <t>provide controls for adjusting forecast recruitments, includes recent mean and multiplier on R0 and others</t>
   </si>
 </sst>
 </file>
@@ -831,8 +840,8 @@
   <dimension ref="A1:G364"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A28" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="F41" sqref="F41"/>
+      <pane ySplit="3" topLeftCell="A35" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -854,7 +863,7 @@
         <v>8</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25"/>
@@ -1663,19 +1672,51 @@
         <v>54</v>
       </c>
       <c r="F41" s="9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G41" s="5" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A42" s="15"/>
-      <c r="F42" s="9"/>
-    </row>
-    <row r="43" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A43" s="15"/>
-      <c r="F43" s="9"/>
+      <c r="A42" s="15">
+        <v>43056</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F42" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="G42" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A43" s="15">
+        <v>43059</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F43" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="G43" s="5" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="44" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="15"/>

</xml_diff>

<commit_message>
VLAB #45838 fix bug in calc of settlement age
</commit_message>
<xml_diff>
--- a/SS_330_Change_Log.xlsx
+++ b/SS_330_Change_Log.xlsx
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="117">
   <si>
     <t>Date</t>
   </si>
@@ -386,9 +386,6 @@
     <t>improve some warnings and adjust array dimensions to allow very long forecasts</t>
   </si>
   <si>
-    <t>2017-11-20 for 3.30.09.00</t>
-  </si>
-  <si>
     <t>3.30.09.00</t>
   </si>
   <si>
@@ -396,6 +393,30 @@
   </si>
   <si>
     <t>provide controls for adjusting forecast recruitments, includes recent mean and multiplier on R0 and others</t>
+  </si>
+  <si>
+    <t>provide controls for bycatch fleets</t>
+  </si>
+  <si>
+    <t>provide benchmark and forecast option to use F0.1; this is either/or with F(Btgt)</t>
+  </si>
+  <si>
+    <t>clarify internal usage and output for SSB_virgin vs SSB_unfished (benchmark); add description to manual</t>
+  </si>
+  <si>
+    <t>clarify output in forecast-report.sso and SPR/YPR profile</t>
+  </si>
+  <si>
+    <t>3.30.10.00</t>
+  </si>
+  <si>
+    <t>2018-01-25 for 3.30.10.01</t>
+  </si>
+  <si>
+    <t>3.30.10.01</t>
+  </si>
+  <si>
+    <t>fix logic error in calculation of settlement age in 2 season, 2 settlement setup</t>
   </si>
 </sst>
 </file>
@@ -841,7 +862,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A35" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="F40" sqref="F40"/>
+      <selection pane="bottomLeft" activeCell="F50" sqref="F50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -863,7 +884,7 @@
         <v>8</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25"/>
@@ -1683,7 +1704,7 @@
         <v>43056</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C42" s="5" t="s">
         <v>31</v>
@@ -1692,7 +1713,7 @@
         <v>25</v>
       </c>
       <c r="F42" s="9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G42" s="5" t="s">
         <v>92</v>
@@ -1703,7 +1724,7 @@
         <v>43059</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C43" s="5" t="s">
         <v>31</v>
@@ -1712,31 +1733,111 @@
         <v>13</v>
       </c>
       <c r="F43" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G43" s="5" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A44" s="15"/>
-      <c r="F44" s="9"/>
+      <c r="A44" s="15">
+        <v>43066</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="F44" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="G44" s="5" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="45" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A45" s="15"/>
-      <c r="F45" s="9"/>
-    </row>
-    <row r="46" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A46" s="15"/>
-      <c r="F46" s="9"/>
+      <c r="A45" s="15">
+        <v>43066</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F45" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="G45" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A46" s="15">
+        <v>43066</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F46" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="G46" s="5" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="47" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A47" s="15"/>
-      <c r="F47" s="9"/>
+      <c r="A47" s="15">
+        <v>43109</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F47" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="G47" s="5" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="48" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A48" s="15"/>
-      <c r="F48" s="9"/>
+      <c r="A48" s="15">
+        <v>43125</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F48" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="G48" s="5" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="15"/>

</xml_diff>

<commit_message>
preliminary commit of 3.30.11.00
</commit_message>
<xml_diff>
--- a/SS_330_Change_Log.xlsx
+++ b/SS_330_Change_Log.xlsx
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="126">
   <si>
     <t>Date</t>
   </si>
@@ -410,13 +410,40 @@
     <t>3.30.10.00</t>
   </si>
   <si>
-    <t>2018-01-25 for 3.30.10.01</t>
-  </si>
-  <si>
     <t>3.30.10.01</t>
   </si>
   <si>
     <t>fix logic error in calculation of settlement age in 2 season, 2 settlement setup</t>
+  </si>
+  <si>
+    <t>3.30.10.02</t>
+  </si>
+  <si>
+    <t>misc</t>
+  </si>
+  <si>
+    <t>fix problem with super year in generalized size comp</t>
+  </si>
+  <si>
+    <t>break SS_write.tpl into SS_write, SS_write_report and SS_write_ssnew</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> clean-up the cout's at end of run</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> for Richards growth, disable trap on fish shrinkage due to code interaction</t>
+  </si>
+  <si>
+    <t>3.30.11.00</t>
+  </si>
+  <si>
+    <t>2018-02-27 for 3.30.11.00</t>
+  </si>
+  <si>
+    <t>revise format of ss_summary</t>
+  </si>
+  <si>
+    <t>add totbio, smrybio and totcal catch to end of ss_summary, but without se</t>
   </si>
 </sst>
 </file>
@@ -862,7 +889,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A35" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="F50" sqref="F50"/>
+      <selection pane="bottomLeft" activeCell="F54" sqref="F54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -884,7 +911,7 @@
         <v>8</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>114</v>
+        <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25"/>
@@ -1824,7 +1851,7 @@
         <v>43125</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C48" s="5" t="s">
         <v>31</v>
@@ -1833,68 +1860,166 @@
         <v>20</v>
       </c>
       <c r="F48" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="G48" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="15">
+        <v>43133</v>
+      </c>
+      <c r="B49" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="G48" s="5" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="15"/>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="15"/>
-    </row>
-    <row r="51" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="15"/>
-      <c r="F51" s="9"/>
-    </row>
-    <row r="52" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A52" s="15"/>
-      <c r="F52" s="9"/>
-    </row>
-    <row r="53" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="15"/>
-      <c r="F53" s="9"/>
-    </row>
-    <row r="54" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A54" s="15"/>
-      <c r="F54" s="9"/>
-    </row>
-    <row r="55" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C49" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D49" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="F49" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="G49" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="15">
+        <v>43133</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="F50" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="G50" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A51" s="15">
+        <v>43133</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="F51" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="G51" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A52" s="15">
+        <v>43158</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F52" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="G52" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A53" s="15">
+        <v>43158</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D53" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="F53" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="G53" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A54" s="15">
+        <v>43158</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F54" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="G54" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" s="15"/>
       <c r="F55" s="9"/>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="15"/>
     </row>
-    <row r="57" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" s="15"/>
       <c r="F57" s="9"/>
     </row>
-    <row r="58" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58" s="15"/>
       <c r="F58" s="9"/>
     </row>
-    <row r="59" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A59" s="15"/>
       <c r="F59" s="9"/>
     </row>
-    <row r="60" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A60" s="15"/>
       <c r="F60" s="9"/>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="15"/>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="15"/>
     </row>
-    <row r="63" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A63" s="15"/>
       <c r="F63" s="9"/>
     </row>
-    <row r="64" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A64" s="15"/>
       <c r="F64" s="9"/>
     </row>

</xml_diff>

<commit_message>
3.30.11.00 - preliminary version of SRR:  Shepherd and Ricker-Power
</commit_message>
<xml_diff>
--- a/SS_330_Change_Log.xlsx
+++ b/SS_330_Change_Log.xlsx
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="129">
   <si>
     <t>Date</t>
   </si>
@@ -341,9 +341,6 @@
 -9999 0 0  # terminator for list of relF</t>
   </si>
   <si>
-    <t>I/O_Change</t>
-  </si>
-  <si>
     <t>Yes</t>
   </si>
   <si>
@@ -437,13 +434,25 @@
     <t>3.30.11.00</t>
   </si>
   <si>
-    <t>2018-02-27 for 3.30.11.00</t>
-  </si>
-  <si>
     <t>revise format of ss_summary</t>
   </si>
   <si>
     <t>add totbio, smrybio and totcal catch to end of ss_summary, but without se</t>
+  </si>
+  <si>
+    <t>add copyright disclaimer</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> parameter specific labels for double normal selectivity</t>
+  </si>
+  <si>
+    <t>Input_Change?</t>
+  </si>
+  <si>
+    <t>2018-03-09 for 3.30.11.00</t>
+  </si>
+  <si>
+    <t>revise reportdetail in starter.ss so value of 0 omits nearly all output files except ss_summary.sso</t>
   </si>
 </sst>
 </file>
@@ -888,8 +897,8 @@
   <dimension ref="A1:G364"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A35" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="F54" sqref="F54"/>
+      <pane ySplit="3" topLeftCell="A43" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="F62" sqref="F62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -911,7 +920,7 @@
         <v>8</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25"/>
@@ -935,7 +944,7 @@
         <v>6</v>
       </c>
       <c r="G3" s="16" t="s">
-        <v>91</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -947,7 +956,7 @@
         <v>10</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -967,7 +976,7 @@
         <v>11</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -990,7 +999,7 @@
         <v>18</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -1013,7 +1022,7 @@
         <v>22</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
@@ -1036,7 +1045,7 @@
         <v>27</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
@@ -1053,7 +1062,7 @@
         <v>29</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
@@ -1076,7 +1085,7 @@
         <v>33</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
@@ -1096,7 +1105,7 @@
         <v>37</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -1116,7 +1125,7 @@
         <v>36</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1136,7 +1145,7 @@
         <v>39</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -1156,7 +1165,7 @@
         <v>44</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -1176,7 +1185,7 @@
         <v>47</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -1196,7 +1205,7 @@
         <v>45</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -1219,7 +1228,7 @@
         <v>48</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -1242,7 +1251,7 @@
         <v>51</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
@@ -1265,7 +1274,7 @@
         <v>53</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
@@ -1285,7 +1294,7 @@
         <v>55</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -1305,7 +1314,7 @@
         <v>72</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -1325,7 +1334,7 @@
         <v>73</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -1345,7 +1354,7 @@
         <v>60</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
@@ -1365,7 +1374,7 @@
         <v>71</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -1385,7 +1394,7 @@
         <v>62</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -1408,7 +1417,7 @@
         <v>64</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -1431,7 +1440,7 @@
         <v>65</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -1454,7 +1463,7 @@
         <v>67</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -1477,7 +1486,7 @@
         <v>68</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
@@ -1497,7 +1506,7 @@
         <v>70</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -1520,7 +1529,7 @@
         <v>76</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -1543,7 +1552,7 @@
         <v>79</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -1563,7 +1572,7 @@
         <v>81</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="110.25" x14ac:dyDescent="0.25">
@@ -1583,7 +1592,7 @@
         <v>90</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -1603,7 +1612,7 @@
         <v>86</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -1623,7 +1632,7 @@
         <v>88</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -1643,7 +1652,7 @@
         <v>89</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -1651,19 +1660,19 @@
         <v>43007</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F38" s="9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G38" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -1671,7 +1680,7 @@
         <v>43045</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>12</v>
@@ -1680,10 +1689,10 @@
         <v>13</v>
       </c>
       <c r="F39" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -1691,7 +1700,7 @@
         <v>43046</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>31</v>
@@ -1700,10 +1709,10 @@
         <v>69</v>
       </c>
       <c r="F40" s="9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -1711,7 +1720,7 @@
         <v>43046</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>24</v>
@@ -1720,10 +1729,10 @@
         <v>54</v>
       </c>
       <c r="F41" s="9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -1731,7 +1740,7 @@
         <v>43056</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C42" s="5" t="s">
         <v>31</v>
@@ -1740,10 +1749,10 @@
         <v>25</v>
       </c>
       <c r="F42" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G42" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
@@ -1751,7 +1760,7 @@
         <v>43059</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C43" s="5" t="s">
         <v>31</v>
@@ -1760,10 +1769,10 @@
         <v>13</v>
       </c>
       <c r="F43" s="9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -1771,7 +1780,7 @@
         <v>43066</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C44" s="5" t="s">
         <v>31</v>
@@ -1780,10 +1789,10 @@
         <v>82</v>
       </c>
       <c r="F44" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G44" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -1791,7 +1800,7 @@
         <v>43066</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C45" s="5" t="s">
         <v>31</v>
@@ -1800,10 +1809,10 @@
         <v>13</v>
       </c>
       <c r="F45" s="9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
@@ -1811,7 +1820,7 @@
         <v>43066</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C46" s="5" t="s">
         <v>31</v>
@@ -1820,10 +1829,10 @@
         <v>13</v>
       </c>
       <c r="F46" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G46" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -1831,7 +1840,7 @@
         <v>43109</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C47" s="5" t="s">
         <v>31</v>
@@ -1840,10 +1849,10 @@
         <v>13</v>
       </c>
       <c r="F47" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -1851,7 +1860,7 @@
         <v>43125</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C48" s="5" t="s">
         <v>31</v>
@@ -1860,10 +1869,10 @@
         <v>20</v>
       </c>
       <c r="F48" s="9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
@@ -1871,7 +1880,7 @@
         <v>43133</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C49" s="5" t="s">
         <v>12</v>
@@ -1880,10 +1889,10 @@
         <v>54</v>
       </c>
       <c r="F49" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
@@ -1891,19 +1900,19 @@
         <v>43133</v>
       </c>
       <c r="B50" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C50" s="5" t="s">
         <v>116</v>
-      </c>
-      <c r="C50" s="5" t="s">
-        <v>117</v>
       </c>
       <c r="D50" s="5" t="s">
         <v>54</v>
       </c>
       <c r="F50" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G50" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -1911,19 +1920,19 @@
         <v>43133</v>
       </c>
       <c r="B51" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C51" s="5" t="s">
         <v>116</v>
-      </c>
-      <c r="C51" s="5" t="s">
-        <v>117</v>
       </c>
       <c r="D51" s="5" t="s">
         <v>54</v>
       </c>
       <c r="F51" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G51" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -1931,7 +1940,7 @@
         <v>43158</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C52" s="5" t="s">
         <v>12</v>
@@ -1940,10 +1949,10 @@
         <v>43</v>
       </c>
       <c r="F52" s="9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G52" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -1951,19 +1960,19 @@
         <v>43158</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C53" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F53" s="9" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -1971,31 +1980,80 @@
         <v>43158</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>43</v>
+        <v>100</v>
       </c>
       <c r="F54" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="G54" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A55" s="15">
+        <v>43158</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D55" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="F55" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="G55" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" s="15">
+        <v>43165</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D56" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="F56" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="G56" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" s="15">
+        <v>43166</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D57" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="F57" s="15" t="s">
         <v>125</v>
       </c>
-      <c r="G54" s="5" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A55" s="15"/>
-      <c r="F55" s="9"/>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="15"/>
-    </row>
-    <row r="57" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A57" s="15"/>
-      <c r="F57" s="9"/>
+      <c r="G57" s="5" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="58" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58" s="15"/>
@@ -2020,11 +2078,9 @@
       <c r="F63" s="9"/>
     </row>
     <row r="64" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A64" s="15"/>
       <c r="F64" s="9"/>
     </row>
     <row r="65" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A65" s="15"/>
       <c r="F65" s="9"/>
     </row>
     <row r="66" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
3.30.11.00; rearrange code to allow usage of -noest
</commit_message>
<xml_diff>
--- a/SS_330_Change_Log.xlsx
+++ b/SS_330_Change_Log.xlsx
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="133">
   <si>
     <t>Date</t>
   </si>
@@ -449,10 +449,22 @@
     <t>Input_Change?</t>
   </si>
   <si>
-    <t>2018-03-09 for 3.30.11.00</t>
-  </si>
-  <si>
     <t>revise reportdetail in starter.ss so value of 0 omits nearly all output files except ss_summary.sso</t>
+  </si>
+  <si>
+    <t>2018-03-26 for 3.30.11.00</t>
+  </si>
+  <si>
+    <t>Ricker power spawner-recruitment; see Cope and Punt (2017)</t>
+  </si>
+  <si>
+    <t>re-arrange code to allow -noest option to work; note that -maxfn 0 -phase 99  also works to bypass estimation</t>
+  </si>
+  <si>
+    <t>add spawner-recruitment plotting output below spawn_recr in report.sso</t>
+  </si>
+  <si>
+    <t>controls</t>
   </si>
 </sst>
 </file>
@@ -898,7 +910,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A37" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="A49" sqref="A49:F49"/>
+      <selection pane="bottomLeft" activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -920,7 +932,7 @@
         <v>8</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25"/>
@@ -2029,7 +2041,7 @@
         <v>100</v>
       </c>
       <c r="F56" s="15" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G56" s="5" t="s">
         <v>92</v>
@@ -2055,17 +2067,65 @@
         <v>92</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A58" s="15"/>
-      <c r="F58" s="9"/>
-    </row>
-    <row r="59" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A59" s="15"/>
-      <c r="F59" s="9"/>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" s="15">
+        <v>43169</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="F58" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="G58" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" s="15">
+        <v>43185</v>
+      </c>
+      <c r="B59" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="C59" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D59" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="F59" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="G59" s="5" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="60" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A60" s="15"/>
-      <c r="F60" s="9"/>
+      <c r="A60" s="15">
+        <v>43185</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="C60" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="F60" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="G60" s="5" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="15"/>

</xml_diff>

<commit_message>
still 3.30.11.00; VLAB#48308; #48236; #45394 for start-up of MCMC and outputing expected surveys to ss_summary in ln()
</commit_message>
<xml_diff>
--- a/SS_330_Change_Log.xlsx
+++ b/SS_330_Change_Log.xlsx
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="138">
   <si>
     <t>Date</t>
   </si>
@@ -452,9 +452,6 @@
     <t>revise reportdetail in starter.ss so value of 0 omits nearly all output files except ss_summary.sso</t>
   </si>
   <si>
-    <t>2018-03-26 for 3.30.11.00</t>
-  </si>
-  <si>
     <t>Ricker power spawner-recruitment; see Cope and Punt (2017)</t>
   </si>
   <si>
@@ -465,6 +462,24 @@
   </si>
   <si>
     <t>controls</t>
+  </si>
+  <si>
+    <t>Cond</t>
+  </si>
+  <si>
+    <t>MCMC</t>
+  </si>
+  <si>
+    <t>improve treatment of biasadjustment when transitioning into MCMC; include MCMC_bump read from starter.ss</t>
+  </si>
+  <si>
+    <t>2018-03-28 for 3.30.11.00</t>
+  </si>
+  <si>
+    <t>add output of selected estimated survey values to sdreport and show in ss_summary.sso</t>
+  </si>
+  <si>
+    <t>add output of ln(SPB) for 3 years to sdreport and show in ss_summary.sso</t>
   </si>
 </sst>
 </file>
@@ -909,8 +924,8 @@
   <dimension ref="A1:G364"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A37" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="F51" sqref="F51"/>
+      <pane ySplit="3" topLeftCell="A46" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="C66" sqref="C66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -920,7 +935,7 @@
     <col min="3" max="3" width="9.28515625" style="5" customWidth="1"/>
     <col min="4" max="4" width="13" style="5" customWidth="1"/>
     <col min="5" max="5" width="13.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="100" style="6" customWidth="1"/>
+    <col min="6" max="6" width="101.7109375" style="6" customWidth="1"/>
     <col min="7" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
@@ -932,7 +947,7 @@
         <v>8</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25"/>
@@ -2081,7 +2096,7 @@
         <v>69</v>
       </c>
       <c r="F58" s="15" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G58" s="5" t="s">
         <v>92</v>
@@ -2098,10 +2113,10 @@
         <v>31</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F59" s="15" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G59" s="5" t="s">
         <v>92</v>
@@ -2121,21 +2136,71 @@
         <v>100</v>
       </c>
       <c r="F60" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G60" s="5" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61" s="15"/>
+    <row r="61" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A61" s="15">
+        <v>43187</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="C61" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D61" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="F61" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="G61" s="5" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62" s="15"/>
+      <c r="A62" s="15">
+        <v>43187</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="F62" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="G62" s="5" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="63" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A63" s="15"/>
-      <c r="F63" s="9"/>
+      <c r="A63" s="15">
+        <v>43187</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="C63" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D63" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="F63" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="G63" s="5" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="64" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="F64" s="9"/>

</xml_diff>

<commit_message>
commit version log for 3.30.12 on 8/29/2018
</commit_message>
<xml_diff>
--- a/SS_330_Change_Log.xlsx
+++ b/SS_330_Change_Log.xlsx
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="176">
   <si>
     <t>Date</t>
   </si>
@@ -446,9 +446,6 @@
     <t xml:space="preserve"> parameter specific labels for double normal selectivity</t>
   </si>
   <si>
-    <t>Input_Change?</t>
-  </si>
-  <si>
     <t>revise reportdetail in starter.ss so value of 0 omits nearly all output files except ss_summary.sso</t>
   </si>
   <si>
@@ -473,13 +470,130 @@
     <t>improve treatment of biasadjustment when transitioning into MCMC; include MCMC_bump read from starter.ss</t>
   </si>
   <si>
-    <t>2018-03-28 for 3.30.11.00</t>
-  </si>
-  <si>
     <t>add output of selected estimated survey values to sdreport and show in ss_summary.sso</t>
   </si>
   <si>
     <t>add output of ln(SPB) for 3 years to sdreport and show in ss_summary.sso</t>
+  </si>
+  <si>
+    <t>2018-08-29 for 3.30.12.00</t>
+  </si>
+  <si>
+    <t>enhance control rule options to:  Control rule method (1: ramp does catch=f(SSB), buffer on F; 2: ramp does F=f(SSB), buffer on F; 3: ramp does catch=f(SSB), buffer on catch; 4: ramp does F=f(SSB), buffer on catch)</t>
+  </si>
+  <si>
+    <t>Mandatory Input_Change?</t>
+  </si>
+  <si>
+    <t>Yes, if used</t>
+  </si>
+  <si>
+    <t>Mean_Size</t>
+  </si>
+  <si>
+    <t>add column for "type" in mean body size:  #_yr month fleet part type obs stderr;  where type=1 for mean length; type=2 for mean body weight;  replaces use of the sign of partition for indicating type</t>
+  </si>
+  <si>
+    <t>A new age selectivity non-parametric for sex-specific options #44 and #45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">improved error checking on read of wtatage.ss </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Update and explain the usage of the "-1" code for fishery sample timing </t>
+  </si>
+  <si>
+    <t>Changed mean forecast recruitment option to use range of years previously specified in forecast years</t>
+  </si>
+  <si>
+    <t>A fatal warning for len selectivity mirroring of higher numbered fleet</t>
+  </si>
+  <si>
+    <t>improve performance of jitter when parameter are near bounds</t>
+  </si>
+  <si>
+    <t>Bmsy/Bzero has been added to the list of derived quantities</t>
+  </si>
+  <si>
+    <t>Discard-at-age is now reported after catch_at_age in report.sso</t>
+  </si>
+  <si>
+    <t>improve</t>
+  </si>
+  <si>
+    <t>Time-vary SRR parms will now work in the forecast; e.g. regime shift on mean recruitment</t>
+  </si>
+  <si>
+    <t>Selectivity Patterns 42 and 43 will now be read correctly</t>
+  </si>
+  <si>
+    <t>Time-vary growth parameters now work with Richards growth function, but there is no trap to prevent  shrinkage</t>
+  </si>
+  <si>
+    <t>Enable transferring parameter dev phase and dev_se from 3.24 format into 3.30 format</t>
+  </si>
+  <si>
+    <t>only calculate selectivity softparmbounds when parameter phase is positive</t>
+  </si>
+  <si>
+    <t>Label lines in the control.ss_new file have been added to improve readability of the parameters</t>
+  </si>
+  <si>
+    <t>There is now better  output to Fit_Len, Fit_Age, Fit_Size for Francis weighting applications, and Durbin-Watson statistic for autocorrelation of devs</t>
+  </si>
+  <si>
+    <t>subseas info is now reported to improve ability to discern when monthly timing of samples has resulted in assignment to a different subseason</t>
+  </si>
+  <si>
+    <t>Fix and enhance reporting the full spawn_recr curve in report.sso (just after the spawn_recr output)</t>
+  </si>
+  <si>
+    <t>Enabled the display of logL for ignored length and age comp observations.</t>
+  </si>
+  <si>
+    <t>Option to report mean F without numbers weighting</t>
+  </si>
+  <si>
+    <t>implement</t>
+  </si>
+  <si>
+    <t>plus_group growth options now include:  value&gt;0 means exponential decay for growth above maxage (value should approximate initial Z; -999 replicates 3.24; -998 to not allow growth above maxage</t>
+  </si>
+  <si>
+    <t>Implement time-varying ageing bias parameters</t>
+  </si>
+  <si>
+    <t>Implement density-dependent environmental effects on parameters; change specification format</t>
+  </si>
+  <si>
+    <t>fecundity-at-age for benchmark when growth is time-varying is no longer being overwritten</t>
+  </si>
+  <si>
+    <t>Benchmark selectivities now use the correct ALK when growth was time-varying</t>
+  </si>
+  <si>
+    <t>discard</t>
+  </si>
+  <si>
+    <t>age_error</t>
+  </si>
+  <si>
+    <t>time_vary</t>
+  </si>
+  <si>
+    <t>density_dependent</t>
+  </si>
+  <si>
+    <t>Create lambda  type 18 for initial equilibrium regime shift</t>
+  </si>
+  <si>
+    <t>composition</t>
+  </si>
+  <si>
+    <t>Allow time-vary R0 tooccur in initial equilibrium year; matches 3.24</t>
+  </si>
+  <si>
+    <t>3.30.12.00</t>
   </si>
 </sst>
 </file>
@@ -586,7 +700,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -615,7 +729,12 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -924,8 +1043,8 @@
   <dimension ref="A1:G364"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A46" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="C66" sqref="C66"/>
+      <pane ySplit="3" topLeftCell="A66" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="F73" sqref="F73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -936,7 +1055,8 @@
     <col min="4" max="4" width="13" style="5" customWidth="1"/>
     <col min="5" max="5" width="13.28515625" style="5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="101.7109375" style="6" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="5"/>
+    <col min="7" max="7" width="14.28515625" style="5" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.35">
@@ -947,11 +1067,11 @@
         <v>8</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -971,7 +1091,7 @@
         <v>6</v>
       </c>
       <c r="G3" s="16" t="s">
-        <v>126</v>
+        <v>138</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -2056,7 +2176,7 @@
         <v>100</v>
       </c>
       <c r="F56" s="15" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G56" s="5" t="s">
         <v>92</v>
@@ -2096,7 +2216,7 @@
         <v>69</v>
       </c>
       <c r="F58" s="15" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G58" s="5" t="s">
         <v>92</v>
@@ -2113,10 +2233,10 @@
         <v>31</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F59" s="15" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G59" s="5" t="s">
         <v>92</v>
@@ -2136,7 +2256,7 @@
         <v>100</v>
       </c>
       <c r="F60" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G60" s="5" t="s">
         <v>92</v>
@@ -2153,13 +2273,13 @@
         <v>24</v>
       </c>
       <c r="D61" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="F61" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="F61" s="9" t="s">
-        <v>134</v>
-      </c>
       <c r="G61" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
@@ -2173,10 +2293,10 @@
         <v>24</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F62" s="6" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="G62" s="5" t="s">
         <v>92</v>
@@ -2193,124 +2313,525 @@
         <v>24</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F63" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="G63" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="15">
+        <v>43341</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="C64" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D64" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F64" s="9" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" s="15">
+        <v>43341</v>
+      </c>
+      <c r="B65" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="C65" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D65" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F65" s="6" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66" s="15">
+        <v>43341</v>
+      </c>
+      <c r="B66" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="C66" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D66" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="F66" s="6" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A67" s="15">
+        <v>43341</v>
+      </c>
+      <c r="B67" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="C67" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D67" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F67" s="6" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68" s="15">
+        <v>43341</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="C68" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D68" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="F68" s="6" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A69" s="15">
+        <v>43341</v>
+      </c>
+      <c r="B69" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="C69" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="D69" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="E69" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="F69" s="9" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" s="15">
+        <v>43341</v>
+      </c>
+      <c r="B70" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="C70" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="D70" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="E70" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="F70" s="6" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A71" s="15">
+        <v>43341</v>
+      </c>
+      <c r="B71" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="C71" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="D71" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F71" s="9" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A72" s="15">
+        <v>43341</v>
+      </c>
+      <c r="B72" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="C72" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="D72" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="F72" s="9" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A73" s="15">
+        <v>43341</v>
+      </c>
+      <c r="B73" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="C73" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="D73" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F73" s="9" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74" s="15">
+        <v>43341</v>
+      </c>
+      <c r="B74" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="C74" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="D74" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F74" s="6" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A75" s="15">
+        <v>43341</v>
+      </c>
+      <c r="B75" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="C75" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="D75" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F75" s="9" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76" s="15">
+        <v>43341</v>
+      </c>
+      <c r="B76" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="C76" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="D76" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="F76" s="6" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A77" s="15">
+        <v>43341</v>
+      </c>
+      <c r="B77" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="C77" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="D77" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F77" s="6" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A78" s="15">
+        <v>43341</v>
+      </c>
+      <c r="B78" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="C78" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D78" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F78" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="G63" s="5" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="F64" s="9"/>
-    </row>
-    <row r="65" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="F65" s="9"/>
-    </row>
-    <row r="66" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A66" s="15"/>
-      <c r="F66" s="9"/>
-    </row>
-    <row r="67" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A67" s="15"/>
-      <c r="F67" s="9"/>
-    </row>
-    <row r="68" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A68" s="15"/>
-      <c r="F68" s="9"/>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="15"/>
-    </row>
-    <row r="70" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A70" s="15"/>
-      <c r="F70" s="9"/>
-    </row>
-    <row r="71" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A71" s="15"/>
-      <c r="F71" s="9"/>
-    </row>
-    <row r="72" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A72" s="15"/>
-      <c r="F72" s="9"/>
-    </row>
-    <row r="73" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A73" s="15"/>
-      <c r="F73" s="9"/>
-    </row>
-    <row r="74" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A74" s="15"/>
-      <c r="F74" s="9"/>
-    </row>
-    <row r="75" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A75" s="15"/>
-      <c r="F75" s="9"/>
-    </row>
-    <row r="76" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A76" s="15"/>
-      <c r="F76" s="9"/>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77" s="15"/>
-    </row>
-    <row r="78" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A78" s="15"/>
-      <c r="F78" s="9"/>
-    </row>
-    <row r="79" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A79" s="15"/>
-      <c r="F79" s="9"/>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A80" s="15"/>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A81" s="15"/>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A82" s="15"/>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A83" s="15"/>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A84" s="15"/>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A85" s="15"/>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A86" s="15"/>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A87" s="15"/>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A88" s="15"/>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A89" s="15"/>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A90" s="15"/>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A91" s="15"/>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="G78" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A79" s="15">
+        <v>43341</v>
+      </c>
+      <c r="B79" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="C79" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D79" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="F79" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="G79" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A80" s="15">
+        <v>43341</v>
+      </c>
+      <c r="B80" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="C80" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D80" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F80" s="9" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A81" s="15">
+        <v>43341</v>
+      </c>
+      <c r="B81" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="C81" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D81" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="F81" s="9" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A82" s="15">
+        <v>43341</v>
+      </c>
+      <c r="B82" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="C82" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D82" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="E82" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="F82" s="9" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A83" s="15">
+        <v>43341</v>
+      </c>
+      <c r="B83" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="C83" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D83" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="F83" s="6" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84" s="15">
+        <v>43341</v>
+      </c>
+      <c r="B84" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="C84" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D84" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="F84" s="6" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85" s="15">
+        <v>43341</v>
+      </c>
+      <c r="B85" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="C85" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D85" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="F85" s="6" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86" s="15">
+        <v>43341</v>
+      </c>
+      <c r="B86" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="C86" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D86" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="F86" s="17" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87" s="15">
+        <v>43341</v>
+      </c>
+      <c r="B87" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="C87" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D87" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="E87" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="F87" s="6" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A88" s="15">
+        <v>43341</v>
+      </c>
+      <c r="B88" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="C88" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D88" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="E88" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="F88" s="9" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A89" s="15">
+        <v>43341</v>
+      </c>
+      <c r="B89" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="C89" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D89" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F89" s="9" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A90" s="15">
+        <v>43341</v>
+      </c>
+      <c r="B90" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="C90" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D90" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="F90" s="6" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A91" s="15">
+        <v>43341</v>
+      </c>
+      <c r="B91" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="C91" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D91" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F91" s="6" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="15"/>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="15"/>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="15"/>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="15"/>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="15"/>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
@@ -3412,9 +3933,8 @@
     </row>
   </sheetData>
   <autoFilter ref="B3:E217"/>
-  <sortState ref="A4:G99">
-    <sortCondition ref="A4:A99"/>
-    <sortCondition ref="B4:B99"/>
+  <sortState ref="C64:G91">
+    <sortCondition ref="E64:E91"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
final commit for 3.30.12 on 2018-09-13
</commit_message>
<xml_diff>
--- a/SS_330_Change_Log.xlsx
+++ b/SS_330_Change_Log.xlsx
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="178">
   <si>
     <t>Date</t>
   </si>
@@ -476,15 +476,9 @@
     <t>add output of ln(SPB) for 3 years to sdreport and show in ss_summary.sso</t>
   </si>
   <si>
-    <t>2018-08-29 for 3.30.12.00</t>
-  </si>
-  <si>
     <t>enhance control rule options to:  Control rule method (1: ramp does catch=f(SSB), buffer on F; 2: ramp does F=f(SSB), buffer on F; 3: ramp does catch=f(SSB), buffer on catch; 4: ramp does F=f(SSB), buffer on catch)</t>
   </si>
   <si>
-    <t>Mandatory Input_Change?</t>
-  </si>
-  <si>
     <t>Yes, if used</t>
   </si>
   <si>
@@ -590,10 +584,22 @@
     <t>composition</t>
   </si>
   <si>
-    <t>Allow time-vary R0 tooccur in initial equilibrium year; matches 3.24</t>
-  </si>
-  <si>
     <t>3.30.12.00</t>
+  </si>
+  <si>
+    <t>2018-09-13 for 3.30.12.00</t>
+  </si>
+  <si>
+    <t>small tweak to parameter jitter and now output the jittering to echoinput.sso</t>
+  </si>
+  <si>
+    <t>begin compiliation with ADMB 12.0</t>
+  </si>
+  <si>
+    <t>Allow time-vary R0 to occur in initial equilibrium year; matches 3.24</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Input_Change?</t>
   </si>
 </sst>
 </file>
@@ -1043,8 +1049,8 @@
   <dimension ref="A1:G364"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A66" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="F73" sqref="F73"/>
+      <pane ySplit="3" topLeftCell="A80" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="G91" sqref="G91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1067,7 +1073,7 @@
         <v>8</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>136</v>
+        <v>173</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25"/>
@@ -1091,7 +1097,7 @@
         <v>6</v>
       </c>
       <c r="G3" s="16" t="s">
-        <v>138</v>
+        <v>177</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -2327,7 +2333,7 @@
         <v>43341</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C64" s="5" t="s">
         <v>12</v>
@@ -2336,7 +2342,7 @@
         <v>13</v>
       </c>
       <c r="F64" s="9" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
@@ -2344,7 +2350,7 @@
         <v>43341</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C65" s="5" t="s">
         <v>12</v>
@@ -2353,7 +2359,7 @@
         <v>25</v>
       </c>
       <c r="F65" s="6" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
@@ -2361,7 +2367,7 @@
         <v>43341</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C66" s="5" t="s">
         <v>12</v>
@@ -2370,7 +2376,7 @@
         <v>75</v>
       </c>
       <c r="F66" s="6" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="67" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -2378,7 +2384,7 @@
         <v>43341</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C67" s="5" t="s">
         <v>12</v>
@@ -2387,7 +2393,7 @@
         <v>43</v>
       </c>
       <c r="F67" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
@@ -2395,7 +2401,7 @@
         <v>43341</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C68" s="5" t="s">
         <v>12</v>
@@ -2404,7 +2410,7 @@
         <v>75</v>
       </c>
       <c r="F68" s="6" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="69" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -2412,19 +2418,19 @@
         <v>43341</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C69" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="D69" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="E69" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="F69" s="9" t="s">
         <v>162</v>
-      </c>
-      <c r="D69" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="E69" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="F69" s="9" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
@@ -2432,19 +2438,19 @@
         <v>43341</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D70" s="5" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E70" s="5" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F70" s="6" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="71" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -2452,16 +2458,16 @@
         <v>43341</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C71" s="5" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D71" s="5" t="s">
         <v>20</v>
       </c>
       <c r="F71" s="9" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="72" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -2469,16 +2475,16 @@
         <v>43341</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C72" s="5" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D72" s="5" t="s">
         <v>82</v>
       </c>
       <c r="F72" s="9" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="73" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -2486,16 +2492,16 @@
         <v>43341</v>
       </c>
       <c r="B73" s="5" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C73" s="5" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D73" s="5" t="s">
         <v>20</v>
       </c>
       <c r="F73" s="9" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
@@ -2503,16 +2509,16 @@
         <v>43341</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C74" s="5" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D74" s="5" t="s">
         <v>20</v>
       </c>
       <c r="F74" s="6" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="75" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -2520,16 +2526,16 @@
         <v>43341</v>
       </c>
       <c r="B75" s="5" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C75" s="5" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D75" s="5" t="s">
         <v>35</v>
       </c>
       <c r="F75" s="9" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
@@ -2537,16 +2543,16 @@
         <v>43341</v>
       </c>
       <c r="B76" s="5" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C76" s="5" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D76" s="5" t="s">
         <v>100</v>
       </c>
       <c r="F76" s="6" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
@@ -2554,16 +2560,16 @@
         <v>43341</v>
       </c>
       <c r="B77" s="5" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C77" s="5" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D77" s="5" t="s">
         <v>20</v>
       </c>
       <c r="F77" s="6" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="78" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
@@ -2571,7 +2577,7 @@
         <v>43341</v>
       </c>
       <c r="B78" s="5" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C78" s="5" t="s">
         <v>24</v>
@@ -2580,10 +2586,10 @@
         <v>13</v>
       </c>
       <c r="F78" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="G78" s="5" t="s">
         <v>137</v>
-      </c>
-      <c r="G78" s="5" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="79" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
@@ -2591,19 +2597,19 @@
         <v>43341</v>
       </c>
       <c r="B79" s="5" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C79" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D79" s="5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F79" s="9" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G79" s="5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="80" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -2611,7 +2617,7 @@
         <v>43341</v>
       </c>
       <c r="B80" s="5" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C80" s="5" t="s">
         <v>31</v>
@@ -2620,15 +2626,18 @@
         <v>25</v>
       </c>
       <c r="F80" s="9" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+      <c r="G80" s="5" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A81" s="15">
         <v>43341</v>
       </c>
       <c r="B81" s="5" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C81" s="5" t="s">
         <v>31</v>
@@ -2637,15 +2646,18 @@
         <v>69</v>
       </c>
       <c r="F81" s="9" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+        <v>170</v>
+      </c>
+      <c r="G81" s="5" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A82" s="15">
         <v>43341</v>
       </c>
       <c r="B82" s="5" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C82" s="5" t="s">
         <v>49</v>
@@ -2654,18 +2666,18 @@
         <v>100</v>
       </c>
       <c r="E82" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="F82" s="9" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A83" s="15">
         <v>43341</v>
       </c>
       <c r="B83" s="5" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C83" s="5" t="s">
         <v>49</v>
@@ -2674,15 +2686,15 @@
         <v>100</v>
       </c>
       <c r="F83" s="6" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="15">
         <v>43341</v>
       </c>
       <c r="B84" s="5" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C84" s="5" t="s">
         <v>49</v>
@@ -2691,15 +2703,15 @@
         <v>100</v>
       </c>
       <c r="F84" s="6" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="15">
         <v>43341</v>
       </c>
       <c r="B85" s="5" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C85" s="5" t="s">
         <v>49</v>
@@ -2708,15 +2720,15 @@
         <v>100</v>
       </c>
       <c r="F85" s="6" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="15">
         <v>43341</v>
       </c>
       <c r="B86" s="5" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C86" s="5" t="s">
         <v>49</v>
@@ -2725,15 +2737,15 @@
         <v>100</v>
       </c>
       <c r="F86" s="17" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="15">
         <v>43341</v>
       </c>
       <c r="B87" s="5" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C87" s="5" t="s">
         <v>49</v>
@@ -2742,18 +2754,18 @@
         <v>100</v>
       </c>
       <c r="E87" s="5" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F87" s="6" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A88" s="15">
         <v>43341</v>
       </c>
       <c r="B88" s="5" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C88" s="5" t="s">
         <v>24</v>
@@ -2765,15 +2777,18 @@
         <v>77</v>
       </c>
       <c r="F88" s="9" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+      <c r="G88" s="5" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A89" s="15">
         <v>43341</v>
       </c>
       <c r="B89" s="5" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C89" s="5" t="s">
         <v>24</v>
@@ -2782,15 +2797,15 @@
         <v>13</v>
       </c>
       <c r="F89" s="9" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="15">
         <v>43341</v>
       </c>
       <c r="B90" s="5" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C90" s="5" t="s">
         <v>24</v>
@@ -2799,15 +2814,15 @@
         <v>69</v>
       </c>
       <c r="F90" s="6" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A91" s="15">
         <v>43341</v>
       </c>
       <c r="B91" s="5" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C91" s="5" t="s">
         <v>24</v>
@@ -2816,22 +2831,50 @@
         <v>43</v>
       </c>
       <c r="F91" s="6" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A92" s="15"/>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A93" s="15"/>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+        <v>161</v>
+      </c>
+      <c r="G91" s="5" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A92" s="15">
+        <v>43356</v>
+      </c>
+      <c r="B92" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="C92" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D92" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="F92" s="6" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A93" s="15">
+        <v>43356</v>
+      </c>
+      <c r="B93" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="C93" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F93" s="6" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="15"/>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="15"/>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="15"/>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
final commit for 3.30.13_beta; fixes F_reporting=5
</commit_message>
<xml_diff>
--- a/SS_330_Change_Log.xlsx
+++ b/SS_330_Change_Log.xlsx
@@ -17,8 +17,8 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$3:$E$217</definedName>
-    <definedName name="_xlnm.database">Sheet1!$A$3:$F$102</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$3:$E$216</definedName>
+    <definedName name="_xlnm.database">Sheet1!$A$3:$F$101</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="199">
   <si>
     <t>Date</t>
   </si>
@@ -587,9 +587,6 @@
     <t>3.30.12.00</t>
   </si>
   <si>
-    <t>2018-09-13 for 3.30.12.00</t>
-  </si>
-  <si>
     <t>small tweak to parameter jitter and now output the jittering to echoinput.sso</t>
   </si>
   <si>
@@ -600,6 +597,72 @@
   </si>
   <si>
     <t xml:space="preserve"> Input_Change?</t>
+  </si>
+  <si>
+    <t>small</t>
+  </si>
+  <si>
+    <t>tag</t>
+  </si>
+  <si>
+    <t>3.30.13.00</t>
+  </si>
+  <si>
+    <t>fix formatting problem for tags output in compreport.sso</t>
+  </si>
+  <si>
+    <t>create new Q option so that mirror Q uses an offset to ln(Q)</t>
+  </si>
+  <si>
+    <t>revise warning for recrdist options</t>
+  </si>
+  <si>
+    <t>small fix to posteriors.sso for Q parms</t>
+  </si>
+  <si>
+    <t>first commit for growth cessation model</t>
+  </si>
+  <si>
+    <t>move tag recapture calculations into a function in SS_tagrep.tpl</t>
+  </si>
+  <si>
+    <t>fix issue with calc of float Q that may have been source of some poor convergences</t>
+  </si>
+  <si>
+    <t>BIG fix with implementation of age-specific K</t>
+  </si>
+  <si>
+    <t>fix implementation of seasons as pseudo-years</t>
+  </si>
+  <si>
+    <t>fix ss_trans to handle mirror q better</t>
+  </si>
+  <si>
+    <t>improve implementation of float q</t>
+  </si>
+  <si>
+    <t>fix reporting when using seasonal MGparms</t>
+  </si>
+  <si>
+    <t>fix output of Dirichlet parameters</t>
+  </si>
+  <si>
+    <t>add dev vector options so last dev can persist to end of time series (codes 21, 22, 23, 24)</t>
+  </si>
+  <si>
+    <t>fix reading of sizecomp obs before styr</t>
+  </si>
+  <si>
+    <t>add new recdev approaches based on dev being relative to R0, not SRR; add column to spawn_recr in report.sso</t>
+  </si>
+  <si>
+    <t>fix output of equilibrium F when using F_reporting=5</t>
+  </si>
+  <si>
+    <t>2018-12-26 for 3.30.13.00</t>
+  </si>
+  <si>
+    <t>internal</t>
   </si>
 </sst>
 </file>
@@ -1046,11 +1109,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:G364"/>
+  <dimension ref="A1:I363"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A80" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="F92" sqref="F92"/>
+      <pane ySplit="3" topLeftCell="A85" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="G109" sqref="G109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1062,7 +1125,8 @@
     <col min="5" max="5" width="13.28515625" style="5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="101.7109375" style="6" customWidth="1"/>
     <col min="7" max="7" width="14.28515625" style="5" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="5"/>
+    <col min="8" max="8" width="12.5703125" style="5" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.35">
@@ -1073,7 +1137,7 @@
         <v>8</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>173</v>
+        <v>197</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25"/>
@@ -1097,7 +1161,7 @@
         <v>6</v>
       </c>
       <c r="G3" s="16" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -2814,7 +2878,7 @@
         <v>69</v>
       </c>
       <c r="F90" s="6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="91" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -2851,7 +2915,7 @@
         <v>78</v>
       </c>
       <c r="F92" s="6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
@@ -2864,70 +2928,336 @@
       <c r="C93" s="5" t="s">
         <v>24</v>
       </c>
+      <c r="D93" s="5" t="s">
+        <v>198</v>
+      </c>
       <c r="F93" s="6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A94" s="15"/>
+      <c r="A94" s="8">
+        <v>43388</v>
+      </c>
+      <c r="B94" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="C94" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D94" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="F94" s="5" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A95" s="15"/>
+      <c r="A95" s="8">
+        <v>43388</v>
+      </c>
+      <c r="B95" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="C95" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D95" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F95" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="G95" s="5" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A96" s="15"/>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A97" s="15"/>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A98" s="15"/>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A99" s="15"/>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A100" s="15"/>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A101" s="15"/>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A102" s="15"/>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A103" s="15"/>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A104" s="15"/>
-    </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A105" s="15"/>
-      <c r="F105" s="3"/>
-    </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A106" s="15"/>
-    </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A107" s="15"/>
-    </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A108" s="15"/>
-    </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A109" s="15"/>
-    </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A110" s="15"/>
-    </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A111" s="15"/>
-    </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A96" s="8">
+        <v>43388</v>
+      </c>
+      <c r="B96" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="C96" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D96" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="F96" s="5" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A97" s="8">
+        <v>43388</v>
+      </c>
+      <c r="B97" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="C97" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="D97" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="F97" s="5" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A98" s="8">
+        <v>43399</v>
+      </c>
+      <c r="B98" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="C98" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D98" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F98" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="G98" s="5" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A99" s="8">
+        <v>43399</v>
+      </c>
+      <c r="B99" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="C99" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D99" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="F99" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="I99" s="8"/>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A100" s="8">
+        <v>43399</v>
+      </c>
+      <c r="B100" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="C100" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D100" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F100" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="I100" s="8"/>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A101" s="8">
+        <v>43411</v>
+      </c>
+      <c r="B101" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="C101" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D101" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F101" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="I101" s="8"/>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A102" s="8">
+        <v>43411</v>
+      </c>
+      <c r="B102" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="C102" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D102" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="F102" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="I102" s="8"/>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A103" s="8">
+        <v>43411</v>
+      </c>
+      <c r="B103" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="C103" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D103" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F103" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="I103" s="8"/>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A104" s="8">
+        <v>43411</v>
+      </c>
+      <c r="B104" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="C104" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D104" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F104" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="I104" s="8"/>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A105" s="8">
+        <v>43412</v>
+      </c>
+      <c r="B105" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="C105" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D105" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="F105" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="I105" s="8"/>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A106" s="8">
+        <v>43440</v>
+      </c>
+      <c r="B106" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="C106" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D106" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="F106" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="I106" s="8"/>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A107" s="8">
+        <v>43446</v>
+      </c>
+      <c r="B107" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="C107" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D107" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="F107" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="G107" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="I107" s="8"/>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A108" s="8">
+        <v>43448</v>
+      </c>
+      <c r="B108" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="C108" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D108" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="F108" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="I108" s="8"/>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A109" s="8">
+        <v>43454</v>
+      </c>
+      <c r="B109" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="C109" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D109" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="F109" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="G109" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="I109" s="8"/>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A110" s="8">
+        <v>43454</v>
+      </c>
+      <c r="B110" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="C110" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D110" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="F110" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="I110" s="8"/>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A111" s="8"/>
+      <c r="I111" s="8"/>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" s="15"/>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" s="15"/>
+      <c r="F113" s="3"/>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" s="15"/>
@@ -2935,6 +3265,7 @@
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" s="15"/>
+      <c r="B115"/>
       <c r="F115" s="3"/>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
@@ -2965,526 +3296,437 @@
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" s="15"/>
       <c r="B121"/>
-      <c r="C121"/>
       <c r="F121" s="3"/>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" s="15"/>
       <c r="B122"/>
-      <c r="C122"/>
       <c r="F122" s="3"/>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" s="15"/>
       <c r="B123"/>
-      <c r="C123"/>
+      <c r="D123"/>
+      <c r="E123"/>
       <c r="F123" s="3"/>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" s="15"/>
       <c r="B124"/>
-      <c r="C124"/>
-      <c r="D124"/>
-      <c r="E124"/>
       <c r="F124" s="3"/>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A125" s="15"/>
+      <c r="A125" s="8"/>
       <c r="B125"/>
-      <c r="C125"/>
       <c r="F125" s="3"/>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" s="8"/>
       <c r="B126"/>
-      <c r="C126"/>
       <c r="F126" s="3"/>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" s="8"/>
       <c r="B127"/>
-      <c r="C127"/>
       <c r="F127" s="3"/>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" s="8"/>
       <c r="B128"/>
-      <c r="C128"/>
       <c r="F128" s="3"/>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" s="8"/>
       <c r="B129"/>
-      <c r="C129"/>
       <c r="F129" s="3"/>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" s="8"/>
       <c r="B130"/>
-      <c r="C130"/>
       <c r="F130" s="3"/>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" s="8"/>
       <c r="B131"/>
-      <c r="C131"/>
       <c r="F131" s="3"/>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" s="8"/>
       <c r="B132"/>
-      <c r="C132"/>
       <c r="F132" s="3"/>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" s="8"/>
       <c r="B133"/>
-      <c r="C133"/>
       <c r="F133" s="3"/>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" s="8"/>
       <c r="B134"/>
-      <c r="C134"/>
       <c r="F134" s="3"/>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135" s="8"/>
       <c r="B135"/>
-      <c r="C135"/>
       <c r="F135" s="3"/>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136" s="8"/>
       <c r="B136"/>
-      <c r="C136"/>
       <c r="F136" s="3"/>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" s="8"/>
       <c r="B137"/>
-      <c r="C137"/>
       <c r="F137" s="3"/>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" s="8"/>
       <c r="B138"/>
-      <c r="C138"/>
       <c r="F138" s="3"/>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" s="8"/>
       <c r="B139"/>
-      <c r="C139"/>
       <c r="F139" s="3"/>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140" s="8"/>
       <c r="B140"/>
-      <c r="C140"/>
       <c r="F140" s="3"/>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" s="8"/>
       <c r="B141"/>
-      <c r="C141"/>
       <c r="F141" s="3"/>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142" s="8"/>
       <c r="B142"/>
-      <c r="C142"/>
       <c r="F142" s="3"/>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143" s="8"/>
       <c r="B143"/>
-      <c r="C143"/>
       <c r="F143" s="3"/>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" s="8"/>
       <c r="B144"/>
-      <c r="C144"/>
       <c r="F144" s="3"/>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145" s="8"/>
       <c r="B145"/>
-      <c r="C145"/>
       <c r="F145" s="3"/>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146" s="8"/>
       <c r="B146"/>
-      <c r="C146"/>
       <c r="F146" s="3"/>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A147" s="8"/>
       <c r="B147"/>
-      <c r="C147"/>
       <c r="F147" s="3"/>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A148" s="8"/>
       <c r="B148"/>
-      <c r="C148"/>
       <c r="F148" s="3"/>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A149" s="8"/>
       <c r="B149"/>
-      <c r="C149"/>
       <c r="F149" s="3"/>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A150" s="8"/>
       <c r="B150"/>
-      <c r="C150"/>
       <c r="F150" s="3"/>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A151" s="8"/>
       <c r="B151"/>
-      <c r="C151"/>
       <c r="F151" s="3"/>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A152" s="8"/>
       <c r="B152"/>
-      <c r="C152"/>
       <c r="F152" s="3"/>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A153" s="8"/>
       <c r="B153"/>
-      <c r="C153"/>
       <c r="F153" s="3"/>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A154" s="8"/>
       <c r="B154"/>
-      <c r="C154"/>
       <c r="F154" s="3"/>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A155" s="8"/>
       <c r="B155"/>
-      <c r="C155"/>
       <c r="F155" s="3"/>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A156" s="8"/>
       <c r="B156"/>
-      <c r="C156"/>
       <c r="F156" s="3"/>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A157" s="8"/>
       <c r="B157"/>
-      <c r="C157"/>
       <c r="F157" s="3"/>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A158" s="8"/>
       <c r="B158"/>
-      <c r="C158"/>
       <c r="F158" s="3"/>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A159" s="8"/>
       <c r="B159"/>
-      <c r="C159"/>
       <c r="F159" s="3"/>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A160" s="8"/>
       <c r="B160"/>
-      <c r="C160"/>
       <c r="F160" s="3"/>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A161" s="8"/>
       <c r="B161"/>
-      <c r="C161"/>
       <c r="F161" s="3"/>
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A162" s="8"/>
       <c r="B162"/>
-      <c r="C162"/>
       <c r="F162" s="3"/>
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A163" s="8"/>
       <c r="B163"/>
-      <c r="C163"/>
       <c r="F163" s="3"/>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A164" s="8"/>
       <c r="B164"/>
-      <c r="C164"/>
       <c r="F164" s="3"/>
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A165" s="8"/>
       <c r="B165"/>
-      <c r="C165"/>
       <c r="F165" s="3"/>
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A166" s="8"/>
       <c r="B166"/>
-      <c r="C166"/>
       <c r="F166" s="3"/>
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A167" s="8"/>
       <c r="B167"/>
-      <c r="C167"/>
       <c r="F167" s="3"/>
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A168" s="8"/>
       <c r="B168"/>
-      <c r="C168"/>
       <c r="F168" s="3"/>
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A169" s="8"/>
       <c r="B169"/>
-      <c r="C169"/>
       <c r="F169" s="3"/>
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A170" s="8"/>
       <c r="B170"/>
-      <c r="C170"/>
       <c r="F170" s="3"/>
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A171" s="8"/>
       <c r="B171"/>
-      <c r="C171"/>
       <c r="F171" s="3"/>
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A172" s="8"/>
       <c r="B172"/>
-      <c r="C172"/>
       <c r="F172" s="3"/>
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A173" s="8"/>
       <c r="B173"/>
-      <c r="C173"/>
       <c r="F173" s="3"/>
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A174" s="8"/>
       <c r="B174"/>
-      <c r="C174"/>
       <c r="F174" s="3"/>
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A175" s="8"/>
       <c r="B175"/>
-      <c r="C175"/>
       <c r="F175" s="3"/>
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A176" s="8"/>
       <c r="B176"/>
-      <c r="C176"/>
       <c r="F176" s="3"/>
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A177" s="8"/>
       <c r="B177"/>
-      <c r="C177"/>
       <c r="F177" s="3"/>
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A178" s="8"/>
       <c r="B178"/>
-      <c r="C178"/>
       <c r="F178" s="3"/>
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A179" s="8"/>
       <c r="B179"/>
-      <c r="C179"/>
       <c r="F179" s="3"/>
     </row>
     <row r="180" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A180" s="8"/>
       <c r="B180"/>
-      <c r="C180"/>
       <c r="F180" s="3"/>
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A181" s="8"/>
       <c r="B181"/>
-      <c r="C181"/>
       <c r="F181" s="3"/>
     </row>
     <row r="182" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A182" s="8"/>
       <c r="B182"/>
-      <c r="C182"/>
       <c r="F182" s="3"/>
     </row>
     <row r="183" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A183" s="8"/>
       <c r="B183"/>
-      <c r="C183"/>
       <c r="F183" s="3"/>
     </row>
     <row r="184" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A184" s="8"/>
       <c r="B184"/>
-      <c r="C184"/>
       <c r="F184" s="3"/>
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A185" s="8"/>
       <c r="B185"/>
-      <c r="C185"/>
       <c r="F185" s="3"/>
     </row>
     <row r="186" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A186" s="8"/>
       <c r="B186"/>
-      <c r="C186"/>
       <c r="F186" s="3"/>
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A187" s="8"/>
       <c r="B187"/>
-      <c r="C187"/>
       <c r="F187" s="3"/>
     </row>
     <row r="188" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A188" s="8"/>
       <c r="B188"/>
-      <c r="C188"/>
       <c r="F188" s="3"/>
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A189" s="8"/>
       <c r="B189"/>
-      <c r="C189"/>
       <c r="F189" s="3"/>
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A190" s="8"/>
       <c r="B190"/>
-      <c r="C190"/>
       <c r="F190" s="3"/>
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A191" s="8"/>
       <c r="B191"/>
-      <c r="C191"/>
       <c r="F191" s="3"/>
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A192" s="8"/>
       <c r="B192"/>
-      <c r="C192"/>
       <c r="F192" s="3"/>
     </row>
     <row r="193" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A193" s="8"/>
       <c r="B193"/>
-      <c r="C193"/>
       <c r="F193" s="3"/>
     </row>
     <row r="194" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A194" s="8"/>
       <c r="B194"/>
-      <c r="C194"/>
       <c r="F194" s="3"/>
     </row>
     <row r="195" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A195" s="8"/>
       <c r="B195"/>
-      <c r="C195"/>
       <c r="F195" s="3"/>
     </row>
     <row r="196" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A196" s="8"/>
       <c r="B196"/>
-      <c r="C196"/>
       <c r="F196" s="3"/>
     </row>
     <row r="197" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A197" s="8"/>
       <c r="B197"/>
-      <c r="C197"/>
       <c r="F197" s="3"/>
     </row>
     <row r="198" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A198" s="8"/>
       <c r="B198"/>
-      <c r="C198"/>
       <c r="F198" s="3"/>
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A199" s="8"/>
       <c r="B199"/>
-      <c r="C199"/>
       <c r="F199" s="3"/>
     </row>
     <row r="200" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A200" s="8"/>
       <c r="B200"/>
-      <c r="C200"/>
       <c r="F200" s="3"/>
     </row>
     <row r="201" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A201" s="8"/>
       <c r="B201"/>
-      <c r="C201"/>
       <c r="F201" s="3"/>
     </row>
     <row r="202" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A202" s="8"/>
       <c r="B202"/>
-      <c r="C202"/>
       <c r="F202" s="3"/>
     </row>
     <row r="203" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A203" s="8"/>
       <c r="B203"/>
-      <c r="C203"/>
       <c r="F203" s="3"/>
     </row>
     <row r="204" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A204" s="8"/>
       <c r="B204"/>
-      <c r="C204"/>
       <c r="F204" s="3"/>
     </row>
     <row r="205" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A205" s="8"/>
       <c r="B205"/>
-      <c r="C205"/>
       <c r="F205" s="3"/>
     </row>
     <row r="206" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A206" s="8"/>
       <c r="B206"/>
-      <c r="C206"/>
       <c r="F206" s="3"/>
     </row>
     <row r="207" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A207" s="8"/>
-      <c r="B207"/>
-      <c r="C207"/>
-      <c r="F207" s="3"/>
     </row>
     <row r="208" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A208" s="8"/>
@@ -3508,30 +3750,30 @@
       <c r="A214" s="8"/>
     </row>
     <row r="215" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A215" s="8"/>
+      <c r="A215" s="13"/>
     </row>
     <row r="216" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A216" s="13"/>
+      <c r="A216" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B216" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C216" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D216" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E216" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F216" s="12" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="217" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A217" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B217" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C217" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D217" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E217" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="F217" s="12" t="s">
-        <v>7</v>
-      </c>
+      <c r="A217" s="8"/>
     </row>
     <row r="218" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A218" s="8"/>
@@ -3971,11 +4213,8 @@
     <row r="363" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A363" s="8"/>
     </row>
-    <row r="364" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A364" s="8"/>
-    </row>
   </sheetData>
-  <autoFilter ref="B3:E217"/>
+  <autoFilter ref="B3:E216"/>
   <sortState ref="C64:G91">
     <sortCondition ref="E64:E91"/>
   </sortState>

</xml_diff>

<commit_message>
Initial commit for 3.30.13.00
</commit_message>
<xml_diff>
--- a/SS_330_Change_Log.xlsx
+++ b/SS_330_Change_Log.xlsx
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="201">
   <si>
     <t>Date</t>
   </si>
@@ -599,9 +599,6 @@
     <t xml:space="preserve"> Input_Change?</t>
   </si>
   <si>
-    <t>small</t>
-  </si>
-  <si>
     <t>tag</t>
   </si>
   <si>
@@ -620,27 +617,15 @@
     <t>small fix to posteriors.sso for Q parms</t>
   </si>
   <si>
-    <t>first commit for growth cessation model</t>
-  </si>
-  <si>
-    <t>move tag recapture calculations into a function in SS_tagrep.tpl</t>
-  </si>
-  <si>
     <t>fix issue with calc of float Q that may have been source of some poor convergences</t>
   </si>
   <si>
-    <t>BIG fix with implementation of age-specific K</t>
-  </si>
-  <si>
     <t>fix implementation of seasons as pseudo-years</t>
   </si>
   <si>
     <t>fix ss_trans to handle mirror q better</t>
   </si>
   <si>
-    <t>improve implementation of float q</t>
-  </si>
-  <si>
     <t>fix reporting when using seasonal MGparms</t>
   </si>
   <si>
@@ -653,16 +638,37 @@
     <t>fix reading of sizecomp obs before styr</t>
   </si>
   <si>
-    <t>add new recdev approaches based on dev being relative to R0, not SRR; add column to spawn_recr in report.sso</t>
-  </si>
-  <si>
     <t>fix output of equilibrium F when using F_reporting=5</t>
   </si>
   <si>
-    <t>2018-12-26 for 3.30.13.00</t>
-  </si>
-  <si>
     <t>internal</t>
+  </si>
+  <si>
+    <t>move tag recapture code into a separate file for ease in future updating:  SS_tagrep.tpl</t>
+  </si>
+  <si>
+    <t>fix issues with F_reporting=4 and 5 for multiseason models</t>
+  </si>
+  <si>
+    <t>add new forecast feature:  year-specific ABC buffer</t>
+  </si>
+  <si>
+    <t>add table for F in report.sso</t>
+  </si>
+  <si>
+    <t>2019-03-08 for 3.30.13.00</t>
+  </si>
+  <si>
+    <t>re-order and organize the list of tables appearing at top of report.sso</t>
+  </si>
+  <si>
+    <t>Important: corrected the -logL calculation for parameter deviations</t>
+  </si>
+  <si>
+    <t>add growth cessation model per Maunder et al (2018)</t>
+  </si>
+  <si>
+    <t>add new recdev approach based on dev being relative to R0, not SRR; add column to spawn_recr in report.sso</t>
   </si>
 </sst>
 </file>
@@ -673,7 +679,7 @@
     <numFmt numFmtId="164" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
     <numFmt numFmtId="165" formatCode="[$-10409]yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -731,6 +737,13 @@
       <name val="Verdana"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -769,7 +782,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -804,6 +817,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1112,8 +1126,8 @@
   <dimension ref="A1:I363"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A85" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="G109" sqref="G109"/>
+      <pane ySplit="3" topLeftCell="A96" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="F98" sqref="F98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1137,7 +1151,7 @@
         <v>8</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25"/>
@@ -2929,253 +2943,238 @@
         <v>24</v>
       </c>
       <c r="D93" s="5" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="F93" s="6" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A94" s="8">
-        <v>43388</v>
-      </c>
-      <c r="B94" s="5" t="s">
+      <c r="A94" s="15"/>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A95" s="15">
+        <v>43532</v>
+      </c>
+      <c r="B95" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="C95" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D95" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="F95" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="C94" s="5" t="s">
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A96" s="15">
+        <v>43532</v>
+      </c>
+      <c r="B96" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="C96" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D94" s="5" t="s">
+      <c r="D96" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F96" s="5" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A97" s="15">
+        <v>43532</v>
+      </c>
+      <c r="B97" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="F94" s="5" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A95" s="8">
-        <v>43388</v>
-      </c>
-      <c r="B95" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="C95" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D95" s="5" t="s">
+      <c r="C97" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D97" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="F97" s="5" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A98" s="15">
+        <v>43532</v>
+      </c>
+      <c r="B98" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="C98" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D98" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F95" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="G95" s="5" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A96" s="8">
-        <v>43388</v>
-      </c>
-      <c r="B96" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="C96" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D96" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="F96" s="5" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A97" s="8">
-        <v>43388</v>
-      </c>
-      <c r="B97" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="C97" s="5" t="s">
-        <v>177</v>
-      </c>
-      <c r="D97" s="5" t="s">
+      <c r="F98" s="5" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A99" s="15">
+        <v>43532</v>
+      </c>
+      <c r="B99" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="C99" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D99" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="F97" s="5" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A98" s="8">
-        <v>43399</v>
-      </c>
-      <c r="B98" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="C98" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D98" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="F98" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="G98" s="5" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A99" s="8">
-        <v>43399</v>
-      </c>
-      <c r="B99" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="C99" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D99" s="5" t="s">
+      <c r="F99" s="5" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A100" s="15">
+        <v>43532</v>
+      </c>
+      <c r="B100" s="5" t="s">
         <v>178</v>
-      </c>
-      <c r="F99" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="I99" s="8"/>
-    </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A100" s="8">
-        <v>43399</v>
-      </c>
-      <c r="B100" s="5" t="s">
-        <v>179</v>
       </c>
       <c r="C100" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D100" s="5" t="s">
-        <v>59</v>
+        <v>100</v>
       </c>
       <c r="F100" s="5" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="I100" s="8"/>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A101" s="8">
-        <v>43411</v>
+      <c r="A101" s="15">
+        <v>43532</v>
       </c>
       <c r="B101" s="5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C101" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D101" s="5" t="s">
-        <v>43</v>
+        <v>78</v>
       </c>
       <c r="F101" s="5" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="I101" s="8"/>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A102" s="8">
-        <v>43411</v>
+      <c r="A102" s="15">
+        <v>43532</v>
       </c>
       <c r="B102" s="5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C102" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D102" s="5" t="s">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="F102" s="5" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="I102" s="8"/>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A103" s="8">
-        <v>43411</v>
+      <c r="A103" s="15">
+        <v>43532</v>
       </c>
       <c r="B103" s="5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C103" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D103" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="F103" s="18" t="s">
+        <v>193</v>
+      </c>
+      <c r="I103" s="8"/>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A104" s="15">
+        <v>43532</v>
+      </c>
+      <c r="B104" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="C104" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D104" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F104" s="18" t="s">
+        <v>198</v>
+      </c>
+      <c r="I104" s="8"/>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A105" s="15">
+        <v>43532</v>
+      </c>
+      <c r="B105" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="C105" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D105" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F103" s="5" t="s">
-        <v>189</v>
-      </c>
-      <c r="I103" s="8"/>
-    </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A104" s="8">
-        <v>43411</v>
-      </c>
-      <c r="B104" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="C104" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D104" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="F104" s="5" t="s">
-        <v>190</v>
-      </c>
-      <c r="I104" s="8"/>
-    </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A105" s="8">
-        <v>43412</v>
-      </c>
-      <c r="B105" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="C105" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D105" s="5" t="s">
-        <v>100</v>
-      </c>
       <c r="F105" s="5" t="s">
-        <v>191</v>
+        <v>180</v>
+      </c>
+      <c r="G105" s="5" t="s">
+        <v>137</v>
       </c>
       <c r="I105" s="8"/>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A106" s="8">
-        <v>43440</v>
+      <c r="A106" s="15">
+        <v>43532</v>
       </c>
       <c r="B106" s="5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C106" s="5" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="D106" s="5" t="s">
-        <v>100</v>
+        <v>43</v>
       </c>
       <c r="F106" s="5" t="s">
-        <v>192</v>
+        <v>199</v>
+      </c>
+      <c r="G106" s="5" t="s">
+        <v>137</v>
       </c>
       <c r="I106" s="8"/>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A107" s="8">
-        <v>43446</v>
+      <c r="A107" s="15">
+        <v>43532</v>
       </c>
       <c r="B107" s="5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C107" s="5" t="s">
         <v>31</v>
@@ -3184,7 +3183,7 @@
         <v>168</v>
       </c>
       <c r="F107" s="5" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="G107" s="5" t="s">
         <v>137</v>
@@ -3192,38 +3191,41 @@
       <c r="I107" s="8"/>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A108" s="8">
-        <v>43448</v>
+      <c r="A108" s="15">
+        <v>43532</v>
       </c>
       <c r="B108" s="5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C108" s="5" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="D108" s="5" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="F108" s="5" t="s">
-        <v>194</v>
+        <v>200</v>
+      </c>
+      <c r="G108" s="5" t="s">
+        <v>137</v>
       </c>
       <c r="I108" s="8"/>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A109" s="8">
-        <v>43454</v>
+      <c r="A109" s="15">
+        <v>43532</v>
       </c>
       <c r="B109" s="5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C109" s="5" t="s">
         <v>31</v>
       </c>
       <c r="D109" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="F109" s="5" t="s">
-        <v>195</v>
+        <v>13</v>
+      </c>
+      <c r="F109" s="18" t="s">
+        <v>194</v>
       </c>
       <c r="G109" s="5" t="s">
         <v>137</v>
@@ -3231,37 +3233,90 @@
       <c r="I109" s="8"/>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A110" s="8">
-        <v>43454</v>
+      <c r="A110" s="15">
+        <v>43532</v>
       </c>
       <c r="B110" s="5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C110" s="5" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="D110" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="F110" s="5" t="s">
-        <v>196</v>
+      <c r="F110" s="18" t="s">
+        <v>195</v>
       </c>
       <c r="I110" s="8"/>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A111" s="8"/>
-      <c r="I111" s="8"/>
+      <c r="A111" s="15">
+        <v>43532</v>
+      </c>
+      <c r="B111" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="C111" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D111" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="F111" s="5" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A112" s="15"/>
+      <c r="A112" s="15">
+        <v>43532</v>
+      </c>
+      <c r="B112" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="C112" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D112" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="F112" s="5" t="s">
+        <v>192</v>
+      </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A113" s="15"/>
-      <c r="F113" s="3"/>
+      <c r="A113" s="15">
+        <v>43532</v>
+      </c>
+      <c r="B113" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="C113" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D113" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="F113" s="18" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A114" s="15"/>
-      <c r="F114" s="3"/>
+      <c r="A114" s="15">
+        <v>43532</v>
+      </c>
+      <c r="B114" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="C114" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D114" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="F114" s="5" t="s">
+        <v>182</v>
+      </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" s="15"/>
@@ -4215,8 +4270,8 @@
     </row>
   </sheetData>
   <autoFilter ref="B3:E216"/>
-  <sortState ref="C64:G91">
-    <sortCondition ref="E64:E91"/>
+  <sortState ref="A95:G114">
+    <sortCondition ref="C95:C114"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
initial commit of branch for fixes to 3.30.13
</commit_message>
<xml_diff>
--- a/SS_330_Change_Log.xlsx
+++ b/SS_330_Change_Log.xlsx
@@ -1122,12 +1122,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet1"/>
+  <sheetPr codeName="Sheet1" filterMode="1"/>
   <dimension ref="A1:I363"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A96" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="F98" sqref="F98"/>
+      <pane ySplit="3" topLeftCell="A92" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="I97" sqref="I97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1178,7 +1178,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8"/>
       <c r="B4" s="5" t="s">
         <v>9</v>
@@ -1190,7 +1190,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="15">
         <v>42683</v>
       </c>
@@ -1210,7 +1210,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="15">
         <v>42689</v>
       </c>
@@ -1233,7 +1233,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="15">
         <v>42691</v>
       </c>
@@ -1256,7 +1256,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="31.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="15">
         <v>42696</v>
       </c>
@@ -1279,7 +1279,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="31.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="15">
         <v>42838</v>
       </c>
@@ -1296,7 +1296,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="31.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="15">
         <v>42838</v>
       </c>
@@ -1319,7 +1319,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="31.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="15">
         <v>42839</v>
       </c>
@@ -1339,7 +1339,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="15">
         <v>42843</v>
       </c>
@@ -1359,7 +1359,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="15">
         <v>42843</v>
       </c>
@@ -1379,7 +1379,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="15">
         <v>42856</v>
       </c>
@@ -1399,7 +1399,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="15">
         <v>42863</v>
       </c>
@@ -1419,7 +1419,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="15">
         <v>42863</v>
       </c>
@@ -1439,7 +1439,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="15">
         <v>42865</v>
       </c>
@@ -1462,7 +1462,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="15">
         <v>42865</v>
       </c>
@@ -1485,7 +1485,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="31.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="15">
         <v>42878</v>
       </c>
@@ -1508,7 +1508,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="31.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="15">
         <v>42885</v>
       </c>
@@ -1528,7 +1528,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="15">
         <v>42907</v>
       </c>
@@ -1548,7 +1548,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="15">
         <v>42914</v>
       </c>
@@ -1568,7 +1568,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="15">
         <v>42928</v>
       </c>
@@ -1588,7 +1588,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="31.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="15">
         <v>42942</v>
       </c>
@@ -1608,7 +1608,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="15">
         <v>42942</v>
       </c>
@@ -1628,7 +1628,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="15">
         <v>42942</v>
       </c>
@@ -1651,7 +1651,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="15">
         <v>42942</v>
       </c>
@@ -1674,7 +1674,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="15">
         <v>42942</v>
       </c>
@@ -1697,7 +1697,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="15">
         <v>42942</v>
       </c>
@@ -1720,7 +1720,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" ht="31.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="15">
         <v>42943</v>
       </c>
@@ -1740,7 +1740,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="15">
         <v>42954</v>
       </c>
@@ -1763,7 +1763,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="15">
         <v>42954</v>
       </c>
@@ -1786,7 +1786,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="15">
         <v>42962</v>
       </c>
@@ -1806,7 +1806,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="110.25" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" ht="110.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="15">
         <v>42976</v>
       </c>
@@ -1826,7 +1826,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="15">
         <v>42989</v>
       </c>
@@ -1846,7 +1846,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="15">
         <v>42989</v>
       </c>
@@ -1866,7 +1866,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="15">
         <v>42989</v>
       </c>
@@ -1886,7 +1886,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="15">
         <v>43007</v>
       </c>
@@ -1906,7 +1906,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="15">
         <v>43045</v>
       </c>
@@ -1926,7 +1926,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="15">
         <v>43046</v>
       </c>
@@ -1946,7 +1946,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="15">
         <v>43046</v>
       </c>
@@ -1966,7 +1966,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="15">
         <v>43056</v>
       </c>
@@ -1986,7 +1986,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" ht="31.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="15">
         <v>43059</v>
       </c>
@@ -2006,7 +2006,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="15">
         <v>43066</v>
       </c>
@@ -2026,7 +2026,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="15">
         <v>43066</v>
       </c>
@@ -2046,7 +2046,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" ht="31.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="15">
         <v>43066</v>
       </c>
@@ -2066,7 +2066,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="15">
         <v>43109</v>
       </c>
@@ -2086,7 +2086,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="15">
         <v>43125</v>
       </c>
@@ -2106,7 +2106,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="15">
         <v>43133</v>
       </c>
@@ -2126,7 +2126,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="15">
         <v>43133</v>
       </c>
@@ -2146,7 +2146,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="15">
         <v>43133</v>
       </c>
@@ -2166,7 +2166,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="15">
         <v>43158</v>
       </c>
@@ -2186,7 +2186,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="15">
         <v>43158</v>
       </c>
@@ -2206,7 +2206,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="15">
         <v>43158</v>
       </c>
@@ -2226,7 +2226,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="15">
         <v>43158</v>
       </c>
@@ -2246,7 +2246,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="15">
         <v>43165</v>
       </c>
@@ -2266,7 +2266,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="15">
         <v>43166</v>
       </c>
@@ -2286,7 +2286,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="15">
         <v>43169</v>
       </c>
@@ -2306,7 +2306,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="15">
         <v>43185</v>
       </c>
@@ -2326,7 +2326,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="15">
         <v>43185</v>
       </c>
@@ -2346,7 +2346,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" ht="31.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="15">
         <v>43187</v>
       </c>
@@ -2366,7 +2366,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="15">
         <v>43187</v>
       </c>
@@ -2386,7 +2386,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="15">
         <v>43187</v>
       </c>
@@ -2406,7 +2406,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="64" spans="1:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" ht="31.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="15">
         <v>43341</v>
       </c>
@@ -2423,7 +2423,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="15">
         <v>43341</v>
       </c>
@@ -2440,7 +2440,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="15">
         <v>43341</v>
       </c>
@@ -2457,7 +2457,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="15">
         <v>43341</v>
       </c>
@@ -2474,7 +2474,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="15">
         <v>43341</v>
       </c>
@@ -2491,7 +2491,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="69" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="15">
         <v>43341</v>
       </c>
@@ -2511,7 +2511,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="15">
         <v>43341</v>
       </c>
@@ -2531,7 +2531,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="71" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="15">
         <v>43341</v>
       </c>
@@ -2548,7 +2548,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="72" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="15">
         <v>43341</v>
       </c>
@@ -2565,7 +2565,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="73" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="15">
         <v>43341</v>
       </c>
@@ -2582,7 +2582,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="15">
         <v>43341</v>
       </c>
@@ -2599,7 +2599,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="75" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" s="15">
         <v>43341</v>
       </c>
@@ -2616,7 +2616,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" s="15">
         <v>43341</v>
       </c>
@@ -2633,7 +2633,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="15">
         <v>43341</v>
       </c>
@@ -2650,7 +2650,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="78" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" ht="47.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="15">
         <v>43341</v>
       </c>
@@ -2670,7 +2670,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="79" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" ht="31.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="15">
         <v>43341</v>
       </c>
@@ -2690,7 +2690,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="80" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="15">
         <v>43341</v>
       </c>
@@ -2710,7 +2710,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="81" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="15">
         <v>43341</v>
       </c>
@@ -2730,7 +2730,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="82" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" ht="31.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="15">
         <v>43341</v>
       </c>
@@ -2750,7 +2750,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="83" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="15">
         <v>43341</v>
       </c>
@@ -2767,7 +2767,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="15">
         <v>43341</v>
       </c>
@@ -2784,7 +2784,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" s="15">
         <v>43341</v>
       </c>
@@ -2801,7 +2801,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="15">
         <v>43341</v>
       </c>
@@ -2818,7 +2818,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="15">
         <v>43341</v>
       </c>
@@ -2838,7 +2838,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="88" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="15">
         <v>43341</v>
       </c>
@@ -2861,7 +2861,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="89" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" s="15">
         <v>43341</v>
       </c>
@@ -2878,7 +2878,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" s="15">
         <v>43341</v>
       </c>
@@ -2895,7 +2895,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="91" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" s="15">
         <v>43341</v>
       </c>
@@ -2915,7 +2915,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" s="15">
         <v>43356</v>
       </c>
@@ -2932,7 +2932,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" s="15">
         <v>43356</v>
       </c>
@@ -2949,7 +2949,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" s="15"/>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
@@ -3318,496 +3318,496 @@
         <v>182</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" s="15"/>
       <c r="B115"/>
       <c r="F115" s="3"/>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" s="15"/>
       <c r="B116"/>
       <c r="F116" s="3"/>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" s="15"/>
       <c r="B117"/>
       <c r="F117" s="3"/>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" s="15"/>
       <c r="B118"/>
       <c r="F118" s="3"/>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" s="15"/>
       <c r="B119"/>
       <c r="F119" s="3"/>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" s="15"/>
       <c r="B120"/>
       <c r="F120" s="3"/>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" s="15"/>
       <c r="B121"/>
       <c r="F121" s="3"/>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" s="15"/>
       <c r="B122"/>
       <c r="F122" s="3"/>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" s="15"/>
       <c r="B123"/>
       <c r="D123"/>
       <c r="E123"/>
       <c r="F123" s="3"/>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" s="15"/>
       <c r="B124"/>
       <c r="F124" s="3"/>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" s="8"/>
       <c r="B125"/>
       <c r="F125" s="3"/>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" s="8"/>
       <c r="B126"/>
       <c r="F126" s="3"/>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" s="8"/>
       <c r="B127"/>
       <c r="F127" s="3"/>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" s="8"/>
       <c r="B128"/>
       <c r="F128" s="3"/>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" s="8"/>
       <c r="B129"/>
       <c r="F129" s="3"/>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" s="8"/>
       <c r="B130"/>
       <c r="F130" s="3"/>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" s="8"/>
       <c r="B131"/>
       <c r="F131" s="3"/>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" s="8"/>
       <c r="B132"/>
       <c r="F132" s="3"/>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" s="8"/>
       <c r="B133"/>
       <c r="F133" s="3"/>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" s="8"/>
       <c r="B134"/>
       <c r="F134" s="3"/>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" s="8"/>
       <c r="B135"/>
       <c r="F135" s="3"/>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" s="8"/>
       <c r="B136"/>
       <c r="F136" s="3"/>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" s="8"/>
       <c r="B137"/>
       <c r="F137" s="3"/>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" s="8"/>
       <c r="B138"/>
       <c r="F138" s="3"/>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" s="8"/>
       <c r="B139"/>
       <c r="F139" s="3"/>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" s="8"/>
       <c r="B140"/>
       <c r="F140" s="3"/>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" s="8"/>
       <c r="B141"/>
       <c r="F141" s="3"/>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" s="8"/>
       <c r="B142"/>
       <c r="F142" s="3"/>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" s="8"/>
       <c r="B143"/>
       <c r="F143" s="3"/>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" s="8"/>
       <c r="B144"/>
       <c r="F144" s="3"/>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145" s="8"/>
       <c r="B145"/>
       <c r="F145" s="3"/>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" s="8"/>
       <c r="B146"/>
       <c r="F146" s="3"/>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" s="8"/>
       <c r="B147"/>
       <c r="F147" s="3"/>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" s="8"/>
       <c r="B148"/>
       <c r="F148" s="3"/>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" s="8"/>
       <c r="B149"/>
       <c r="F149" s="3"/>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" s="8"/>
       <c r="B150"/>
       <c r="F150" s="3"/>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" s="8"/>
       <c r="B151"/>
       <c r="F151" s="3"/>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" s="8"/>
       <c r="B152"/>
       <c r="F152" s="3"/>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" s="8"/>
       <c r="B153"/>
       <c r="F153" s="3"/>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" s="8"/>
       <c r="B154"/>
       <c r="F154" s="3"/>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" s="8"/>
       <c r="B155"/>
       <c r="F155" s="3"/>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" s="8"/>
       <c r="B156"/>
       <c r="F156" s="3"/>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" s="8"/>
       <c r="B157"/>
       <c r="F157" s="3"/>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" s="8"/>
       <c r="B158"/>
       <c r="F158" s="3"/>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" s="8"/>
       <c r="B159"/>
       <c r="F159" s="3"/>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" s="8"/>
       <c r="B160"/>
       <c r="F160" s="3"/>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" s="8"/>
       <c r="B161"/>
       <c r="F161" s="3"/>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" s="8"/>
       <c r="B162"/>
       <c r="F162" s="3"/>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" s="8"/>
       <c r="B163"/>
       <c r="F163" s="3"/>
     </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" s="8"/>
       <c r="B164"/>
       <c r="F164" s="3"/>
     </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" s="8"/>
       <c r="B165"/>
       <c r="F165" s="3"/>
     </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" s="8"/>
       <c r="B166"/>
       <c r="F166" s="3"/>
     </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" s="8"/>
       <c r="B167"/>
       <c r="F167" s="3"/>
     </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" s="8"/>
       <c r="B168"/>
       <c r="F168" s="3"/>
     </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" s="8"/>
       <c r="B169"/>
       <c r="F169" s="3"/>
     </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" s="8"/>
       <c r="B170"/>
       <c r="F170" s="3"/>
     </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" s="8"/>
       <c r="B171"/>
       <c r="F171" s="3"/>
     </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" s="8"/>
       <c r="B172"/>
       <c r="F172" s="3"/>
     </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" s="8"/>
       <c r="B173"/>
       <c r="F173" s="3"/>
     </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" s="8"/>
       <c r="B174"/>
       <c r="F174" s="3"/>
     </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175" s="8"/>
       <c r="B175"/>
       <c r="F175" s="3"/>
     </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" s="8"/>
       <c r="B176"/>
       <c r="F176" s="3"/>
     </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" s="8"/>
       <c r="B177"/>
       <c r="F177" s="3"/>
     </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178" s="8"/>
       <c r="B178"/>
       <c r="F178" s="3"/>
     </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179" s="8"/>
       <c r="B179"/>
       <c r="F179" s="3"/>
     </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" s="8"/>
       <c r="B180"/>
       <c r="F180" s="3"/>
     </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181" s="8"/>
       <c r="B181"/>
       <c r="F181" s="3"/>
     </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" s="8"/>
       <c r="B182"/>
       <c r="F182" s="3"/>
     </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183" s="8"/>
       <c r="B183"/>
       <c r="F183" s="3"/>
     </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184" s="8"/>
       <c r="B184"/>
       <c r="F184" s="3"/>
     </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" s="8"/>
       <c r="B185"/>
       <c r="F185" s="3"/>
     </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186" s="8"/>
       <c r="B186"/>
       <c r="F186" s="3"/>
     </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187" s="8"/>
       <c r="B187"/>
       <c r="F187" s="3"/>
     </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188" s="8"/>
       <c r="B188"/>
       <c r="F188" s="3"/>
     </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189" s="8"/>
       <c r="B189"/>
       <c r="F189" s="3"/>
     </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190" s="8"/>
       <c r="B190"/>
       <c r="F190" s="3"/>
     </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191" s="8"/>
       <c r="B191"/>
       <c r="F191" s="3"/>
     </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192" s="8"/>
       <c r="B192"/>
       <c r="F192" s="3"/>
     </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193" s="8"/>
       <c r="B193"/>
       <c r="F193" s="3"/>
     </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A194" s="8"/>
       <c r="B194"/>
       <c r="F194" s="3"/>
     </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195" s="8"/>
       <c r="B195"/>
       <c r="F195" s="3"/>
     </row>
-    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196" s="8"/>
       <c r="B196"/>
       <c r="F196" s="3"/>
     </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A197" s="8"/>
       <c r="B197"/>
       <c r="F197" s="3"/>
     </row>
-    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A198" s="8"/>
       <c r="B198"/>
       <c r="F198" s="3"/>
     </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A199" s="8"/>
       <c r="B199"/>
       <c r="F199" s="3"/>
     </row>
-    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A200" s="8"/>
       <c r="B200"/>
       <c r="F200" s="3"/>
     </row>
-    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201" s="8"/>
       <c r="B201"/>
       <c r="F201" s="3"/>
     </row>
-    <row r="202" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A202" s="8"/>
       <c r="B202"/>
       <c r="F202" s="3"/>
     </row>
-    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A203" s="8"/>
       <c r="B203"/>
       <c r="F203" s="3"/>
     </row>
-    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A204" s="8"/>
       <c r="B204"/>
       <c r="F204" s="3"/>
     </row>
-    <row r="205" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A205" s="8"/>
       <c r="B205"/>
       <c r="F205" s="3"/>
     </row>
-    <row r="206" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A206" s="8"/>
       <c r="B206"/>
       <c r="F206" s="3"/>
     </row>
-    <row r="207" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207" s="8"/>
     </row>
-    <row r="208" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A208" s="8"/>
     </row>
-    <row r="209" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209" s="8"/>
     </row>
-    <row r="210" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210" s="8"/>
     </row>
-    <row r="211" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A211" s="8"/>
     </row>
-    <row r="212" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A212" s="8"/>
     </row>
-    <row r="213" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A213" s="8"/>
     </row>
-    <row r="214" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A214" s="8"/>
     </row>
-    <row r="215" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A215" s="13"/>
     </row>
-    <row r="216" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A216" s="10" t="s">
         <v>7</v>
       </c>
@@ -4269,7 +4269,13 @@
       <c r="A363" s="8"/>
     </row>
   </sheetData>
-  <autoFilter ref="B3:E216"/>
+  <autoFilter ref="B3:E216">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="3.30.13.00"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState ref="A95:G114">
     <sortCondition ref="C95:C114"/>
   </sortState>

</xml_diff>